<commit_message>
removed KL 221750 analysis, left squeleton for spreadsheet
</commit_message>
<xml_diff>
--- a/GS-2015B-Q-27/SDSSJ221750.50-002425.9/analysis/Reduction_Lines_Verification.xlsx
+++ b/GS-2015B-Q-27/SDSSJ221750.50-002425.9/analysis/Reduction_Lines_Verification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="180" windowWidth="15200" windowHeight="14940" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="11820" yWindow="180" windowWidth="15200" windowHeight="14940" tabRatio="1000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="H vacuum" sheetId="1" r:id="rId1"/>
@@ -639,6 +639,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,31 +670,18 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1141,7 +1141,7 @@
     <col min="3" max="3" width="10.83203125" style="5"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="20"/>
-    <col min="6" max="6" width="7.6640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="10" style="24" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="10" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="12" max="12" width="3.83203125" customWidth="1"/>
@@ -1150,21 +1150,21 @@
     <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="B1" s="2"/>
       <c r="C1" s="18"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="44" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
+      <c r="I1" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="44" t="s">
+      <c r="J1" s="52"/>
+      <c r="K1" s="53"/>
+      <c r="M1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
     </row>
     <row r="2" spans="1:15" s="11" customFormat="1" ht="46" thickBot="1">
       <c r="A2" s="11" t="s">
@@ -1367,38 +1367,31 @@
       <c r="C12" s="5">
         <v>21661.200000000001</v>
       </c>
-      <c r="E12" s="20">
-        <v>21668.400000000001</v>
-      </c>
       <c r="F12" s="24">
         <f>E12-$C12</f>
-        <v>7.2000000000007276</v>
+        <v>-21661.200000000001</v>
       </c>
       <c r="G12" s="10">
         <f>ABS(F12)</f>
-        <v>7.2000000000007276</v>
-      </c>
-      <c r="I12" s="20">
-        <v>21672.400000000001</v>
-      </c>
+        <v>21661.200000000001</v>
+      </c>
+      <c r="I12" s="20"/>
       <c r="J12" s="24">
         <f>I12-$C12</f>
-        <v>11.200000000000728</v>
+        <v>-21661.200000000001</v>
       </c>
       <c r="K12" s="10">
         <f>ABS(J12)</f>
-        <v>11.200000000000728</v>
-      </c>
-      <c r="M12" s="20">
-        <v>21674.3</v>
-      </c>
+        <v>21661.200000000001</v>
+      </c>
+      <c r="M12" s="20"/>
       <c r="N12" s="24">
         <f>M12-$C12</f>
-        <v>13.099999999998545</v>
+        <v>-21661.200000000001</v>
       </c>
       <c r="O12" s="10">
         <f>ABS(N12)</f>
-        <v>13.099999999998545</v>
+        <v>21661.200000000001</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1445,38 +1438,31 @@
       <c r="C15" s="5">
         <v>17366.900000000001</v>
       </c>
-      <c r="E15" s="20">
-        <v>17366.900000000001</v>
-      </c>
       <c r="F15" s="24">
         <f t="shared" ref="F15:F20" si="0">E15-$C15</f>
-        <v>0</v>
+        <v>-17366.900000000001</v>
       </c>
       <c r="G15" s="10">
         <f t="shared" ref="G15:G20" si="1">ABS(F15)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="20">
-        <v>17371.3</v>
-      </c>
+        <v>17366.900000000001</v>
+      </c>
+      <c r="I15" s="20"/>
       <c r="J15" s="24">
         <f t="shared" ref="J15:J20" si="2">I15-$C15</f>
-        <v>4.3999999999978172</v>
+        <v>-17366.900000000001</v>
       </c>
       <c r="K15" s="10">
         <f t="shared" ref="K15:K20" si="3">ABS(J15)</f>
-        <v>4.3999999999978172</v>
-      </c>
-      <c r="M15" s="20">
-        <v>17370.8</v>
-      </c>
+        <v>17366.900000000001</v>
+      </c>
+      <c r="M15" s="20"/>
       <c r="N15" s="24">
         <f t="shared" ref="N15:N20" si="4">M15-$C15</f>
-        <v>3.8999999999978172</v>
+        <v>-17366.900000000001</v>
       </c>
       <c r="O15" s="10">
         <f t="shared" ref="O15:O20" si="5">ABS(N15)</f>
-        <v>3.8999999999978172</v>
+        <v>17366.900000000001</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1489,38 +1475,31 @@
       <c r="C16" s="5">
         <v>16811.099999999999</v>
       </c>
-      <c r="E16" s="20">
-        <v>16813.8</v>
-      </c>
       <c r="F16" s="24">
         <f t="shared" si="0"/>
-        <v>2.7000000000007276</v>
+        <v>-16811.099999999999</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" si="1"/>
-        <v>2.7000000000007276</v>
-      </c>
-      <c r="I16" s="20">
-        <v>16817.2</v>
-      </c>
+        <v>16811.099999999999</v>
+      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="24">
         <f t="shared" si="2"/>
-        <v>6.1000000000021828</v>
+        <v>-16811.099999999999</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="3"/>
-        <v>6.1000000000021828</v>
-      </c>
-      <c r="M16" s="20">
-        <v>16815.599999999999</v>
-      </c>
+        <v>16811.099999999999</v>
+      </c>
+      <c r="M16" s="20"/>
       <c r="N16" s="24">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>-16811.099999999999</v>
       </c>
       <c r="O16" s="10">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>16811.099999999999</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1533,38 +1512,31 @@
       <c r="C17" s="5">
         <v>16411.7</v>
       </c>
-      <c r="E17" s="20">
-        <v>16412.2</v>
-      </c>
       <c r="F17" s="24">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>-16411.7</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="20">
-        <v>16414.3</v>
-      </c>
+        <v>16411.7</v>
+      </c>
+      <c r="I17" s="20"/>
       <c r="J17" s="24">
         <f t="shared" si="2"/>
-        <v>2.5999999999985448</v>
+        <v>-16411.7</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="3"/>
-        <v>2.5999999999985448</v>
-      </c>
-      <c r="M17" s="20">
-        <v>16416.2</v>
-      </c>
+        <v>16411.7</v>
+      </c>
+      <c r="M17" s="20"/>
       <c r="N17" s="24">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>-16411.7</v>
       </c>
       <c r="O17" s="10">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>16411.7</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1577,38 +1549,31 @@
       <c r="C18" s="5">
         <v>16113.7</v>
       </c>
-      <c r="E18" s="20">
-        <v>16112.2</v>
-      </c>
       <c r="F18" s="24">
         <f t="shared" si="0"/>
-        <v>-1.5</v>
+        <v>-16113.7</v>
       </c>
       <c r="G18" s="10">
         <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="I18" s="20">
-        <v>16114.1</v>
-      </c>
+        <v>16113.7</v>
+      </c>
+      <c r="I18" s="20"/>
       <c r="J18" s="24">
         <f t="shared" si="2"/>
-        <v>0.3999999999996362</v>
+        <v>-16113.7</v>
       </c>
       <c r="K18" s="10">
         <f t="shared" si="3"/>
-        <v>0.3999999999996362</v>
-      </c>
-      <c r="M18" s="20">
-        <v>16112.7</v>
-      </c>
+        <v>16113.7</v>
+      </c>
+      <c r="M18" s="20"/>
       <c r="N18" s="24">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-16113.7</v>
       </c>
       <c r="O18" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>16113.7</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1621,38 +1586,31 @@
       <c r="C19" s="5">
         <v>15884.9</v>
       </c>
-      <c r="E19" s="20">
-        <v>15885</v>
-      </c>
       <c r="F19" s="24">
         <f t="shared" si="0"/>
-        <v>0.1000000000003638</v>
+        <v>-15884.9</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="1"/>
-        <v>0.1000000000003638</v>
-      </c>
-      <c r="I19" s="20">
-        <v>15889.2</v>
-      </c>
+        <v>15884.9</v>
+      </c>
+      <c r="I19" s="20"/>
       <c r="J19" s="24">
         <f t="shared" si="2"/>
-        <v>4.3000000000010914</v>
+        <v>-15884.9</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="3"/>
-        <v>4.3000000000010914</v>
-      </c>
-      <c r="M19" s="20">
-        <v>15889.1</v>
-      </c>
+        <v>15884.9</v>
+      </c>
+      <c r="M19" s="20"/>
       <c r="N19" s="24">
         <f t="shared" si="4"/>
-        <v>4.2000000000007276</v>
+        <v>-15884.9</v>
       </c>
       <c r="O19" s="10">
         <f t="shared" si="5"/>
-        <v>4.2000000000007276</v>
+        <v>15884.9</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1665,38 +1623,31 @@
       <c r="C20" s="5">
         <v>15705</v>
       </c>
-      <c r="E20" s="20">
-        <v>15712</v>
-      </c>
       <c r="F20" s="24">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-15705</v>
       </c>
       <c r="G20" s="10">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="I20" s="20">
-        <v>15713.3</v>
-      </c>
+        <v>15705</v>
+      </c>
+      <c r="I20" s="20"/>
       <c r="J20" s="24">
         <f t="shared" si="2"/>
-        <v>8.2999999999992724</v>
+        <v>-15705</v>
       </c>
       <c r="K20" s="10">
         <f t="shared" si="3"/>
-        <v>8.2999999999992724</v>
-      </c>
-      <c r="M20" s="20">
-        <v>15713.7</v>
-      </c>
+        <v>15705</v>
+      </c>
+      <c r="M20" s="20"/>
       <c r="N20" s="24">
         <f t="shared" si="4"/>
-        <v>8.7000000000007276</v>
+        <v>-15705</v>
       </c>
       <c r="O20" s="10">
         <f t="shared" si="5"/>
-        <v>8.7000000000007276</v>
+        <v>15705</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2325,33 +2276,33 @@
       </c>
       <c r="F58" s="24">
         <f>AVERAGE(F15:F20,F12)</f>
-        <v>2.2857142857145454</v>
+        <v>-17136.357142857141</v>
       </c>
       <c r="G58" s="10">
         <f>AVERAGE(G15:G20,G12)</f>
-        <v>2.7142857142859742</v>
+        <v>17136.357142857141</v>
       </c>
       <c r="I58" s="20" t="s">
         <v>67</v>
       </c>
       <c r="J58" s="24">
         <f>AVERAGE(J15:J20,J12)</f>
-        <v>5.3285714285713244</v>
+        <v>-17136.357142857141</v>
       </c>
       <c r="K58" s="10">
         <f>AVERAGE(K15:K20,K12)</f>
-        <v>5.3285714285713244</v>
+        <v>17136.357142857141</v>
       </c>
       <c r="M58" s="20" t="s">
         <v>67</v>
       </c>
       <c r="N58" s="24">
         <f>AVERAGE(N15:N20,N12)</f>
-        <v>5.4142857142854028</v>
+        <v>-17136.357142857141</v>
       </c>
       <c r="O58" s="10">
         <f>AVERAGE(O15:O20,O12)</f>
-        <v>5.6999999999996884</v>
+        <v>17136.357142857141</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -2360,33 +2311,33 @@
       </c>
       <c r="F59" s="24">
         <f>STDEV(F15:F20,F12)</f>
-        <v>3.513511335510807</v>
+        <v>2074.4087092126415</v>
       </c>
       <c r="G59" s="10">
         <f>STDEV(G15:G20,G12)</f>
-        <v>3.1376363563616914</v>
+        <v>2074.4087092126415</v>
       </c>
       <c r="I59" s="20" t="s">
         <v>68</v>
       </c>
       <c r="J59" s="24">
         <f>STDEV(J15:J20,J12)</f>
-        <v>3.5952349416578855</v>
+        <v>2074.4087092126415</v>
       </c>
       <c r="K59" s="10">
         <f>STDEV(K15:K20,K12)</f>
-        <v>3.5952349416578855</v>
+        <v>2074.4087092126415</v>
       </c>
       <c r="M59" s="20" t="s">
         <v>68</v>
       </c>
       <c r="N59" s="24">
         <f>STDEV(N15:N20,N12)</f>
-        <v>4.4054619778285584</v>
+        <v>2074.4087092126415</v>
       </c>
       <c r="O59" s="10">
         <f>STDEV(O15:O20,O12)</f>
-        <v>3.9627431576284899</v>
+        <v>2074.4087092126415</v>
       </c>
     </row>
   </sheetData>
@@ -2409,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q74" sqref="Q74"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2423,7 +2374,7 @@
     <col min="6" max="6" width="10.83203125" style="10"/>
     <col min="7" max="7" width="4.5" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="9" customWidth="1"/>
-    <col min="15" max="15" width="4.1640625" style="60" customWidth="1"/>
+    <col min="15" max="15" width="4.1640625" style="50" customWidth="1"/>
     <col min="18" max="18" width="11.5" customWidth="1"/>
     <col min="19" max="19" width="4.5" style="7" customWidth="1"/>
   </cols>
@@ -2431,34 +2382,34 @@
     <row r="1" spans="1:22" s="1" customFormat="1">
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="H1" s="47" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
+      <c r="H1" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="49"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="56"/>
       <c r="K1" s="30"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="44" t="s">
+      <c r="M1" s="57"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="47" t="s">
+      <c r="Q1" s="59"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="48"/>
-      <c r="V1" s="49"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="56"/>
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="46" thickBot="1">
       <c r="A2" s="16" t="s">
@@ -2495,7 +2446,7 @@
       <c r="N2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="57"/>
+      <c r="O2" s="47"/>
       <c r="P2" s="16" t="s">
         <v>66</v>
       </c>
@@ -2529,7 +2480,7 @@
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
-      <c r="O3" s="58"/>
+      <c r="O3" s="48"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
@@ -2555,21 +2506,19 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="58"/>
+      <c r="O4" s="48"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="34"/>
       <c r="R4" s="34"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="43">
-        <v>10832.9</v>
-      </c>
+      <c r="T4" s="43"/>
       <c r="U4" s="24">
         <f t="shared" ref="U4:U16" si="0">T4-$A4</f>
-        <v>1.6999999999989086</v>
+        <v>-10831.2</v>
       </c>
       <c r="V4" s="10">
         <f t="shared" ref="V4:V16" si="1">ABS(U4)</f>
-        <v>1.6999999999989086</v>
+        <v>10831.2</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="32" customFormat="1">
@@ -2589,21 +2538,19 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
-      <c r="O5" s="58"/>
+      <c r="O5" s="48"/>
       <c r="P5" s="34"/>
       <c r="Q5" s="34"/>
       <c r="R5" s="34"/>
       <c r="S5" s="6"/>
-      <c r="T5" s="43">
-        <v>10973.4</v>
-      </c>
+      <c r="T5" s="43"/>
       <c r="U5" s="24">
         <f t="shared" si="0"/>
-        <v>-2.8999999999996362</v>
+        <v>-10976.3</v>
       </c>
       <c r="V5" s="10">
         <f t="shared" si="1"/>
-        <v>2.8999999999996362</v>
+        <v>10976.3</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="32" customFormat="1">
@@ -2623,21 +2570,19 @@
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
       <c r="N6" s="34"/>
-      <c r="O6" s="58"/>
+      <c r="O6" s="48"/>
       <c r="P6" s="34"/>
       <c r="Q6" s="34"/>
       <c r="R6" s="34"/>
       <c r="S6" s="6"/>
-      <c r="T6" s="43">
-        <v>11439.4</v>
-      </c>
+      <c r="T6" s="43"/>
       <c r="U6" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-11436.4</v>
       </c>
       <c r="V6" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>11436.4</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="32" customFormat="1">
@@ -2657,21 +2602,19 @@
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
-      <c r="O7" s="58"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
       <c r="S7" s="6"/>
-      <c r="T7" s="43">
-        <v>11537.1</v>
-      </c>
+      <c r="T7" s="43"/>
       <c r="U7" s="24">
         <f t="shared" si="0"/>
-        <v>-2.3999999999996362</v>
+        <v>-11539.5</v>
       </c>
       <c r="V7" s="10">
         <f t="shared" si="1"/>
-        <v>2.3999999999996362</v>
+        <v>11539.5</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="32" customFormat="1">
@@ -2691,21 +2634,19 @@
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
-      <c r="O8" s="58"/>
+      <c r="O8" s="48"/>
       <c r="P8" s="34"/>
       <c r="Q8" s="34"/>
       <c r="R8" s="34"/>
       <c r="S8" s="6"/>
-      <c r="T8" s="43">
-        <v>11591.4</v>
-      </c>
+      <c r="T8" s="43"/>
       <c r="U8" s="24">
         <f t="shared" si="0"/>
-        <v>-1.1000000000003638</v>
+        <v>-11592.5</v>
       </c>
       <c r="V8" s="10">
         <f t="shared" si="1"/>
-        <v>1.1000000000003638</v>
+        <v>11592.5</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="32" customFormat="1">
@@ -2725,21 +2666,19 @@
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
       <c r="N9" s="34"/>
-      <c r="O9" s="58"/>
+      <c r="O9" s="48"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
       <c r="S9" s="6"/>
-      <c r="T9" s="43">
-        <v>11647.9</v>
-      </c>
+      <c r="T9" s="43"/>
       <c r="U9" s="24">
         <f t="shared" si="0"/>
-        <v>-3.6000000000003638</v>
+        <v>-11651.5</v>
       </c>
       <c r="V9" s="10">
         <f t="shared" si="1"/>
-        <v>3.6000000000003638</v>
+        <v>11651.5</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="32" customFormat="1">
@@ -2759,21 +2698,19 @@
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
       <c r="N10" s="34"/>
-      <c r="O10" s="58"/>
+      <c r="O10" s="48"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="34"/>
       <c r="R10" s="34"/>
       <c r="S10" s="6"/>
-      <c r="T10" s="43">
-        <v>12122.6</v>
-      </c>
+      <c r="T10" s="43"/>
       <c r="U10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-12122.6</v>
       </c>
       <c r="V10" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12122.6</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="32" customFormat="1">
@@ -2793,21 +2730,19 @@
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
-      <c r="O11" s="58"/>
+      <c r="O11" s="48"/>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
       <c r="S11" s="6"/>
-      <c r="T11" s="43">
-        <v>12229</v>
-      </c>
+      <c r="T11" s="43"/>
       <c r="U11" s="24">
         <f t="shared" si="0"/>
-        <v>-0.2999999999992724</v>
+        <v>-12229.3</v>
       </c>
       <c r="V11" s="10">
         <f t="shared" si="1"/>
-        <v>0.2999999999992724</v>
+        <v>12229.3</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="32" customFormat="1">
@@ -2827,21 +2762,19 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="58"/>
+      <c r="O12" s="48"/>
       <c r="P12" s="34"/>
       <c r="Q12" s="34"/>
       <c r="R12" s="34"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="43">
-        <v>12285.9</v>
-      </c>
+      <c r="T12" s="43"/>
       <c r="U12" s="24">
         <f t="shared" si="0"/>
-        <v>-1.1000000000003638</v>
+        <v>-12287</v>
       </c>
       <c r="V12" s="10">
         <f t="shared" si="1"/>
-        <v>1.1000000000003638</v>
+        <v>12287</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="32" customFormat="1">
@@ -2861,21 +2794,19 @@
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="58"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
       <c r="S13" s="6"/>
-      <c r="T13" s="43">
-        <v>12350.8</v>
-      </c>
+      <c r="T13" s="43"/>
       <c r="U13" s="24">
         <f t="shared" si="0"/>
-        <v>-0.80000000000109139</v>
+        <v>-12351.6</v>
       </c>
       <c r="V13" s="10">
         <f t="shared" si="1"/>
-        <v>0.80000000000109139</v>
+        <v>12351.6</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="32" customFormat="1">
@@ -2895,21 +2826,19 @@
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
-      <c r="O14" s="58"/>
+      <c r="O14" s="48"/>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
       <c r="R14" s="34"/>
       <c r="S14" s="6"/>
-      <c r="T14" s="43">
-        <v>12906.4</v>
-      </c>
+      <c r="T14" s="43"/>
       <c r="U14" s="24">
         <f t="shared" si="0"/>
-        <v>0.69999999999890861</v>
+        <v>-12905.7</v>
       </c>
       <c r="V14" s="10">
         <f t="shared" si="1"/>
-        <v>0.69999999999890861</v>
+        <v>12905.7</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="32" customFormat="1">
@@ -2929,21 +2858,19 @@
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="58"/>
+      <c r="O15" s="48"/>
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="43">
-        <v>13020.6</v>
-      </c>
+      <c r="T15" s="43"/>
       <c r="U15" s="24">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-13021.6</v>
       </c>
       <c r="V15" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>13021.6</v>
       </c>
     </row>
     <row r="16" spans="1:22" s="32" customFormat="1">
@@ -2963,21 +2890,19 @@
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
-      <c r="O16" s="58"/>
+      <c r="O16" s="48"/>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="43">
-        <v>13085.3</v>
-      </c>
+      <c r="T16" s="43"/>
       <c r="U16" s="24">
         <f t="shared" si="0"/>
-        <v>9.9999999998544808E-2</v>
+        <v>-13085.2</v>
       </c>
       <c r="V16" s="10">
         <f t="shared" si="1"/>
-        <v>9.9999999998544808E-2</v>
+        <v>13085.2</v>
       </c>
     </row>
     <row r="17" spans="1:22" s="32" customFormat="1">
@@ -2993,7 +2918,7 @@
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
-      <c r="O17" s="58"/>
+      <c r="O17" s="48"/>
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
@@ -3019,21 +2944,19 @@
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
-      <c r="O18" s="58"/>
+      <c r="O18" s="48"/>
       <c r="P18" s="34"/>
       <c r="Q18" s="34"/>
       <c r="R18" s="34"/>
       <c r="S18" s="6"/>
-      <c r="T18" s="43">
-        <v>14357.8</v>
-      </c>
+      <c r="T18" s="43"/>
       <c r="U18" s="24">
         <f t="shared" ref="U18:U25" si="2">T18-$A18</f>
-        <v>13.399999999999636</v>
+        <v>-14344.4</v>
       </c>
       <c r="V18" s="10">
         <f t="shared" ref="V18:V25" si="3">ABS(U18)</f>
-        <v>13.399999999999636</v>
+        <v>14344.4</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="32" customFormat="1">
@@ -3053,21 +2976,19 @@
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
-      <c r="O19" s="58"/>
+      <c r="O19" s="48"/>
       <c r="P19" s="34"/>
       <c r="Q19" s="34"/>
       <c r="R19" s="34"/>
       <c r="S19" s="6"/>
-      <c r="T19" s="43">
-        <v>14520.4</v>
-      </c>
+      <c r="T19" s="43"/>
       <c r="U19" s="24">
         <f t="shared" si="2"/>
-        <v>1.3999999999996362</v>
+        <v>-14519</v>
       </c>
       <c r="V19" s="10">
         <f t="shared" si="3"/>
-        <v>1.3999999999996362</v>
+        <v>14519</v>
       </c>
     </row>
     <row r="20" spans="1:22" s="32" customFormat="1">
@@ -3087,21 +3008,19 @@
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
-      <c r="O20" s="58"/>
+      <c r="O20" s="48"/>
       <c r="P20" s="34"/>
       <c r="Q20" s="34"/>
       <c r="R20" s="34"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="43">
-        <v>14564.7</v>
-      </c>
+      <c r="T20" s="43"/>
       <c r="U20" s="24">
         <f t="shared" si="2"/>
-        <v>0.7000000000007276</v>
+        <v>-14564</v>
       </c>
       <c r="V20" s="10">
         <f t="shared" si="3"/>
-        <v>0.7000000000007276</v>
+        <v>14564</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="32" customFormat="1">
@@ -3121,21 +3040,19 @@
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
-      <c r="O21" s="58"/>
+      <c r="O21" s="48"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
       <c r="R21" s="34"/>
       <c r="S21" s="6"/>
-      <c r="T21" s="43">
-        <v>14606.4</v>
-      </c>
+      <c r="T21" s="43"/>
       <c r="U21" s="24">
         <f t="shared" si="2"/>
-        <v>1.6000000000003638</v>
+        <v>-14604.8</v>
       </c>
       <c r="V21" s="10">
         <f t="shared" si="3"/>
-        <v>1.6000000000003638</v>
+        <v>14604.8</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="32" customFormat="1">
@@ -3155,21 +3072,19 @@
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
-      <c r="O22" s="58"/>
+      <c r="O22" s="48"/>
       <c r="P22" s="34"/>
       <c r="Q22" s="34"/>
       <c r="R22" s="34"/>
       <c r="S22" s="6"/>
-      <c r="T22" s="43">
-        <v>14700</v>
-      </c>
+      <c r="T22" s="43"/>
       <c r="U22" s="24">
         <f t="shared" si="2"/>
-        <v>1.6000000000003638</v>
+        <v>-14698.4</v>
       </c>
       <c r="V22" s="10">
         <f t="shared" si="3"/>
-        <v>1.6000000000003638</v>
+        <v>14698.4</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="32" customFormat="1">
@@ -3189,21 +3104,19 @@
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
-      <c r="O23" s="58"/>
+      <c r="O23" s="48"/>
       <c r="P23" s="34"/>
       <c r="Q23" s="34"/>
       <c r="R23" s="34"/>
       <c r="S23" s="6"/>
-      <c r="T23" s="43">
-        <v>14800.2</v>
-      </c>
+      <c r="T23" s="43"/>
       <c r="U23" s="24">
         <f t="shared" si="2"/>
-        <v>0.40000000000145519</v>
+        <v>-14799.8</v>
       </c>
       <c r="V23" s="10">
         <f t="shared" si="3"/>
-        <v>0.40000000000145519</v>
+        <v>14799.8</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="32" customFormat="1">
@@ -3223,21 +3136,19 @@
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
-      <c r="O24" s="58"/>
+      <c r="O24" s="48"/>
       <c r="P24" s="34"/>
       <c r="Q24" s="34"/>
       <c r="R24" s="34"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="43">
-        <v>14834.2</v>
-      </c>
+      <c r="T24" s="43"/>
       <c r="U24" s="24">
         <f t="shared" si="2"/>
-        <v>1.2000000000007276</v>
+        <v>-14833</v>
       </c>
       <c r="V24" s="10">
         <f t="shared" si="3"/>
-        <v>1.2000000000007276</v>
+        <v>14833</v>
       </c>
     </row>
     <row r="25" spans="1:22" s="32" customFormat="1">
@@ -3257,21 +3168,19 @@
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
       <c r="N25" s="34"/>
-      <c r="O25" s="58"/>
+      <c r="O25" s="48"/>
       <c r="P25" s="34"/>
       <c r="Q25" s="34"/>
       <c r="R25" s="34"/>
       <c r="S25" s="6"/>
-      <c r="T25" s="43">
-        <v>14889.1</v>
-      </c>
+      <c r="T25" s="43"/>
       <c r="U25" s="24">
         <f t="shared" si="2"/>
-        <v>1.3999999999996362</v>
+        <v>-14887.7</v>
       </c>
       <c r="V25" s="10">
         <f t="shared" si="3"/>
-        <v>1.3999999999996362</v>
+        <v>14887.7</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -3282,7 +3191,7 @@
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
-      <c r="O26" s="59"/>
+      <c r="O26" s="49"/>
       <c r="P26" s="24"/>
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
@@ -3297,27 +3206,22 @@
       <c r="B27" s="17">
         <v>1.95</v>
       </c>
-      <c r="D27" s="20">
-        <v>15054.1</v>
-      </c>
       <c r="E27" s="24">
         <f t="shared" ref="E27:E42" si="4">D27-$A27</f>
-        <v>-1.3999999999996362</v>
+        <v>-15055.5</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" ref="F27:F42" si="5">ABS(E27)</f>
-        <v>1.3999999999996362</v>
-      </c>
-      <c r="H27" s="20">
-        <v>15053.8</v>
-      </c>
+        <v>15055.5</v>
+      </c>
+      <c r="H27" s="20"/>
       <c r="I27" s="24">
         <f t="shared" ref="I27:I42" si="6">H27-$A27</f>
-        <v>-1.7000000000007276</v>
+        <v>-15055.5</v>
       </c>
       <c r="J27" s="10">
         <f t="shared" ref="J27:J42" si="7">ABS(I27)</f>
-        <v>1.7000000000007276</v>
+        <v>15055.5</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="20">
@@ -3331,28 +3235,24 @@
         <f t="shared" ref="N27:N42" si="9">ABS(M27)</f>
         <v>0.2999999999992724</v>
       </c>
-      <c r="O27" s="59"/>
-      <c r="P27" s="20">
-        <v>15054.9</v>
-      </c>
+      <c r="O27" s="49"/>
+      <c r="P27" s="20"/>
       <c r="Q27" s="24">
         <f t="shared" ref="Q27:Q42" si="10">P27-$A27</f>
-        <v>-0.6000000000003638</v>
+        <v>-15055.5</v>
       </c>
       <c r="R27" s="24">
         <f t="shared" ref="R27:R42" si="11">ABS(Q27)</f>
-        <v>0.6000000000003638</v>
-      </c>
-      <c r="T27" s="20">
-        <v>15059.9</v>
-      </c>
+        <v>15055.5</v>
+      </c>
+      <c r="T27" s="20"/>
       <c r="U27" s="24">
         <f t="shared" ref="U27:U42" si="12">T27-$A27</f>
-        <v>4.3999999999996362</v>
+        <v>-15055.5</v>
       </c>
       <c r="V27" s="10">
         <f t="shared" ref="V27:V42" si="13">ABS(U27)</f>
-        <v>4.3999999999996362</v>
+        <v>15055.5</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -3362,27 +3262,22 @@
       <c r="B28" s="17">
         <v>1.41</v>
       </c>
-      <c r="D28" s="20">
-        <v>15238.4</v>
-      </c>
       <c r="E28" s="24">
         <f t="shared" si="4"/>
-        <v>-2.6000000000003638</v>
+        <v>-15241</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="5"/>
-        <v>2.6000000000003638</v>
-      </c>
-      <c r="H28" s="20">
-        <v>15239.8</v>
-      </c>
+        <v>15241</v>
+      </c>
+      <c r="H28" s="20"/>
       <c r="I28" s="24">
         <f t="shared" si="6"/>
-        <v>-1.2000000000007276</v>
+        <v>-15241</v>
       </c>
       <c r="J28" s="10">
         <f t="shared" si="7"/>
-        <v>1.2000000000007276</v>
+        <v>15241</v>
       </c>
       <c r="K28" s="10"/>
       <c r="L28" s="20">
@@ -3396,28 +3291,24 @@
         <f t="shared" si="9"/>
         <v>1.2000000000007276</v>
       </c>
-      <c r="O28" s="59"/>
-      <c r="P28" s="20">
-        <v>15240.2</v>
-      </c>
+      <c r="O28" s="49"/>
+      <c r="P28" s="20"/>
       <c r="Q28" s="24">
         <f t="shared" si="10"/>
-        <v>-0.7999999999992724</v>
+        <v>-15241</v>
       </c>
       <c r="R28" s="24">
         <f t="shared" si="11"/>
-        <v>0.7999999999992724</v>
-      </c>
-      <c r="T28" s="20">
-        <v>15242.5</v>
-      </c>
+        <v>15241</v>
+      </c>
+      <c r="T28" s="20"/>
       <c r="U28" s="24">
         <f t="shared" si="12"/>
-        <v>1.5</v>
+        <v>-15241</v>
       </c>
       <c r="V28" s="10">
         <f t="shared" si="13"/>
-        <v>1.5</v>
+        <v>15241</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -3427,27 +3318,22 @@
       <c r="B29" s="17">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D29" s="20">
-        <v>15332.3</v>
-      </c>
       <c r="E29" s="24">
         <f t="shared" si="4"/>
-        <v>-0.1000000000003638</v>
+        <v>-15332.4</v>
       </c>
       <c r="F29" s="10">
         <f t="shared" si="5"/>
-        <v>0.1000000000003638</v>
-      </c>
-      <c r="H29" s="20">
-        <v>15331</v>
-      </c>
+        <v>15332.4</v>
+      </c>
+      <c r="H29" s="20"/>
       <c r="I29" s="24">
         <f t="shared" si="6"/>
-        <v>-1.3999999999996362</v>
+        <v>-15332.4</v>
       </c>
       <c r="J29" s="10">
         <f t="shared" si="7"/>
-        <v>1.3999999999996362</v>
+        <v>15332.4</v>
       </c>
       <c r="K29" s="10"/>
       <c r="L29" s="20">
@@ -3461,28 +3347,24 @@
         <f t="shared" si="9"/>
         <v>1.1999999999989086</v>
       </c>
-      <c r="O29" s="59"/>
-      <c r="P29" s="20">
-        <v>15332</v>
-      </c>
+      <c r="O29" s="49"/>
+      <c r="P29" s="20"/>
       <c r="Q29" s="24">
         <f t="shared" si="10"/>
-        <v>-0.3999999999996362</v>
+        <v>-15332.4</v>
       </c>
       <c r="R29" s="24">
         <f t="shared" si="11"/>
-        <v>0.3999999999996362</v>
-      </c>
-      <c r="T29" s="20">
-        <v>15334.7</v>
-      </c>
+        <v>15332.4</v>
+      </c>
+      <c r="T29" s="20"/>
       <c r="U29" s="24">
         <f t="shared" si="12"/>
-        <v>2.3000000000010914</v>
+        <v>-15332.4</v>
       </c>
       <c r="V29" s="10">
         <f t="shared" si="13"/>
-        <v>2.3000000000010914</v>
+        <v>15332.4</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -3492,27 +3374,22 @@
       <c r="B30" s="17">
         <v>1.08</v>
       </c>
-      <c r="D30" s="20">
-        <v>15430.8</v>
-      </c>
       <c r="E30" s="24">
         <f t="shared" si="4"/>
-        <v>-1.3000000000010914</v>
+        <v>-15432.1</v>
       </c>
       <c r="F30" s="10">
         <f t="shared" si="5"/>
-        <v>1.3000000000010914</v>
-      </c>
-      <c r="H30" s="20">
-        <v>15429.5</v>
-      </c>
+        <v>15432.1</v>
+      </c>
+      <c r="H30" s="20"/>
       <c r="I30" s="24">
         <f t="shared" si="6"/>
-        <v>-2.6000000000003638</v>
+        <v>-15432.1</v>
       </c>
       <c r="J30" s="10">
         <f t="shared" si="7"/>
-        <v>2.6000000000003638</v>
+        <v>15432.1</v>
       </c>
       <c r="K30" s="10"/>
       <c r="L30" s="20">
@@ -3526,28 +3403,24 @@
         <f t="shared" si="9"/>
         <v>0.6000000000003638</v>
       </c>
-      <c r="O30" s="59"/>
-      <c r="P30" s="20">
-        <v>15432.3</v>
-      </c>
+      <c r="O30" s="49"/>
+      <c r="P30" s="20"/>
       <c r="Q30" s="24">
         <f t="shared" si="10"/>
-        <v>0.19999999999890861</v>
+        <v>-15432.1</v>
       </c>
       <c r="R30" s="24">
         <f t="shared" si="11"/>
-        <v>0.19999999999890861</v>
-      </c>
-      <c r="T30" s="20">
-        <v>15434.1</v>
-      </c>
+        <v>15432.1</v>
+      </c>
+      <c r="T30" s="20"/>
       <c r="U30" s="24">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-15432.1</v>
       </c>
       <c r="V30" s="10">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>15432.1</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -3557,27 +3430,22 @@
       <c r="B31" s="17">
         <v>1.05</v>
       </c>
-      <c r="D31" s="20">
-        <v>15652.7</v>
-      </c>
       <c r="E31" s="24">
         <f t="shared" si="4"/>
-        <v>-2.2999999999992724</v>
+        <v>-15655</v>
       </c>
       <c r="F31" s="10">
         <f t="shared" si="5"/>
-        <v>2.2999999999992724</v>
-      </c>
-      <c r="H31" s="20">
-        <v>15652.5</v>
-      </c>
+        <v>15655</v>
+      </c>
+      <c r="H31" s="20"/>
       <c r="I31" s="24">
         <f t="shared" si="6"/>
-        <v>-2.5</v>
+        <v>-15655</v>
       </c>
       <c r="J31" s="10">
         <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>15655</v>
       </c>
       <c r="K31" s="10"/>
       <c r="L31" s="20">
@@ -3591,28 +3459,24 @@
         <f t="shared" si="9"/>
         <v>3.2000000000007276</v>
       </c>
-      <c r="O31" s="59"/>
-      <c r="P31" s="20">
-        <v>15655.7</v>
-      </c>
+      <c r="O31" s="49"/>
+      <c r="P31" s="20"/>
       <c r="Q31" s="24">
         <f t="shared" si="10"/>
-        <v>0.7000000000007276</v>
+        <v>-15655</v>
       </c>
       <c r="R31" s="24">
         <f t="shared" si="11"/>
-        <v>0.7000000000007276</v>
-      </c>
-      <c r="T31" s="20">
-        <v>15656.3</v>
-      </c>
+        <v>15655</v>
+      </c>
+      <c r="T31" s="20"/>
       <c r="U31" s="24">
         <f t="shared" si="12"/>
-        <v>1.2999999999992724</v>
+        <v>-15655</v>
       </c>
       <c r="V31" s="10">
         <f t="shared" si="13"/>
-        <v>1.2999999999992724</v>
+        <v>15655</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -3622,27 +3486,22 @@
       <c r="B32" s="17">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D32" s="20">
-        <v>15833</v>
-      </c>
       <c r="E32" s="24">
         <f t="shared" si="4"/>
-        <v>-0.2000000000007276</v>
+        <v>-15833.2</v>
       </c>
       <c r="F32" s="10">
         <f t="shared" si="5"/>
-        <v>0.2000000000007276</v>
-      </c>
-      <c r="H32" s="20">
-        <v>15832.6</v>
-      </c>
+        <v>15833.2</v>
+      </c>
+      <c r="H32" s="20"/>
       <c r="I32" s="24">
         <f t="shared" si="6"/>
-        <v>-0.6000000000003638</v>
+        <v>-15833.2</v>
       </c>
       <c r="J32" s="10">
         <f t="shared" si="7"/>
-        <v>0.6000000000003638</v>
+        <v>15833.2</v>
       </c>
       <c r="K32" s="10"/>
       <c r="L32" s="20">
@@ -3656,28 +3515,24 @@
         <f t="shared" si="9"/>
         <v>0.2999999999992724</v>
       </c>
-      <c r="O32" s="59"/>
-      <c r="P32" s="20">
-        <v>15834</v>
-      </c>
+      <c r="O32" s="49"/>
+      <c r="P32" s="20"/>
       <c r="Q32" s="24">
         <f t="shared" si="10"/>
-        <v>0.7999999999992724</v>
+        <v>-15833.2</v>
       </c>
       <c r="R32" s="24">
         <f t="shared" si="11"/>
-        <v>0.7999999999992724</v>
-      </c>
-      <c r="T32" s="20">
-        <v>15839.9</v>
-      </c>
+        <v>15833.2</v>
+      </c>
+      <c r="T32" s="20"/>
       <c r="U32" s="24">
         <f t="shared" si="12"/>
-        <v>6.6999999999989086</v>
+        <v>-15833.2</v>
       </c>
       <c r="V32" s="10">
         <f t="shared" si="13"/>
-        <v>6.6999999999989086</v>
+        <v>15833.2</v>
       </c>
     </row>
     <row r="33" spans="1:22">
@@ -3687,27 +3542,22 @@
       <c r="B33" s="17">
         <v>1.53</v>
       </c>
-      <c r="D33" s="20">
-        <v>16030</v>
-      </c>
       <c r="E33" s="24">
         <f t="shared" si="4"/>
-        <v>-0.7999999999992724</v>
+        <v>-16030.8</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" si="5"/>
-        <v>0.7999999999992724</v>
-      </c>
-      <c r="H33" s="20">
-        <v>16029</v>
-      </c>
+        <v>16030.8</v>
+      </c>
+      <c r="H33" s="20"/>
       <c r="I33" s="24">
         <f t="shared" si="6"/>
-        <v>-1.7999999999992724</v>
+        <v>-16030.8</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" si="7"/>
-        <v>1.7999999999992724</v>
+        <v>16030.8</v>
       </c>
       <c r="K33" s="10"/>
       <c r="L33" s="20">
@@ -3721,28 +3571,24 @@
         <f t="shared" si="9"/>
         <v>0.8999999999996362</v>
       </c>
-      <c r="O33" s="59"/>
-      <c r="P33" s="20">
-        <v>16030.2</v>
-      </c>
+      <c r="O33" s="49"/>
+      <c r="P33" s="20"/>
       <c r="Q33" s="24">
         <f t="shared" si="10"/>
-        <v>-0.59999999999854481</v>
+        <v>-16030.8</v>
       </c>
       <c r="R33" s="24">
         <f t="shared" si="11"/>
-        <v>0.59999999999854481</v>
-      </c>
-      <c r="T33" s="20">
-        <v>16033.7</v>
-      </c>
+        <v>16030.8</v>
+      </c>
+      <c r="T33" s="20"/>
       <c r="U33" s="24">
         <f t="shared" si="12"/>
-        <v>2.9000000000014552</v>
+        <v>-16030.8</v>
       </c>
       <c r="V33" s="10">
         <f t="shared" si="13"/>
-        <v>2.9000000000014552</v>
+        <v>16030.8</v>
       </c>
     </row>
     <row r="34" spans="1:22">
@@ -3752,27 +3598,22 @@
       <c r="B34" s="17">
         <v>1.71</v>
       </c>
-      <c r="D34" s="20">
-        <v>16127.8</v>
-      </c>
       <c r="E34" s="24">
         <f t="shared" si="4"/>
-        <v>-0.80000000000109139</v>
+        <v>-16128.6</v>
       </c>
       <c r="F34" s="10">
         <f t="shared" si="5"/>
-        <v>0.80000000000109139</v>
-      </c>
-      <c r="H34" s="20">
-        <v>16126.7</v>
-      </c>
+        <v>16128.6</v>
+      </c>
+      <c r="H34" s="20"/>
       <c r="I34" s="24">
         <f t="shared" si="6"/>
-        <v>-1.8999999999996362</v>
+        <v>-16128.6</v>
       </c>
       <c r="J34" s="10">
         <f t="shared" si="7"/>
-        <v>1.8999999999996362</v>
+        <v>16128.6</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="20">
@@ -3786,28 +3627,24 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="O34" s="59"/>
-      <c r="P34" s="20">
-        <v>16128.7</v>
-      </c>
+      <c r="O34" s="49"/>
+      <c r="P34" s="20"/>
       <c r="Q34" s="24">
         <f t="shared" si="10"/>
-        <v>0.1000000000003638</v>
+        <v>-16128.6</v>
       </c>
       <c r="R34" s="24">
         <f t="shared" si="11"/>
-        <v>0.1000000000003638</v>
-      </c>
-      <c r="T34" s="20">
-        <v>16131.1</v>
-      </c>
+        <v>16128.6</v>
+      </c>
+      <c r="T34" s="20"/>
       <c r="U34" s="24">
         <f t="shared" si="12"/>
-        <v>2.5</v>
+        <v>-16128.6</v>
       </c>
       <c r="V34" s="10">
         <f t="shared" si="13"/>
-        <v>2.5</v>
+        <v>16128.6</v>
       </c>
     </row>
     <row r="35" spans="1:22">
@@ -3817,27 +3654,22 @@
       <c r="B35" s="17">
         <v>1.27</v>
       </c>
-      <c r="D35" s="20">
-        <v>16234.7</v>
-      </c>
       <c r="E35" s="24">
         <f t="shared" si="4"/>
-        <v>-0.69999999999890861</v>
+        <v>-16235.4</v>
       </c>
       <c r="F35" s="10">
         <f t="shared" si="5"/>
-        <v>0.69999999999890861</v>
-      </c>
-      <c r="H35" s="20">
-        <v>16233.2</v>
-      </c>
+        <v>16235.4</v>
+      </c>
+      <c r="H35" s="20"/>
       <c r="I35" s="24">
         <f t="shared" si="6"/>
-        <v>-2.1999999999989086</v>
+        <v>-16235.4</v>
       </c>
       <c r="J35" s="10">
         <f t="shared" si="7"/>
-        <v>2.1999999999989086</v>
+        <v>16235.4</v>
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="20">
@@ -3851,28 +3683,24 @@
         <f t="shared" si="9"/>
         <v>1.2999999999992724</v>
       </c>
-      <c r="O35" s="59"/>
-      <c r="P35" s="20">
-        <v>16234.5</v>
-      </c>
+      <c r="O35" s="49"/>
+      <c r="P35" s="20"/>
       <c r="Q35" s="24">
         <f t="shared" si="10"/>
-        <v>-0.8999999999996362</v>
+        <v>-16235.4</v>
       </c>
       <c r="R35" s="24">
         <f t="shared" si="11"/>
-        <v>0.8999999999996362</v>
-      </c>
-      <c r="T35" s="20">
-        <v>16237.2</v>
-      </c>
+        <v>16235.4</v>
+      </c>
+      <c r="T35" s="20"/>
       <c r="U35" s="24">
         <f t="shared" si="12"/>
-        <v>1.8000000000010914</v>
+        <v>-16235.4</v>
       </c>
       <c r="V35" s="10">
         <f t="shared" si="13"/>
-        <v>1.8000000000010914</v>
+        <v>16235.4</v>
       </c>
     </row>
     <row r="36" spans="1:22">
@@ -3882,27 +3710,22 @@
       <c r="B36" s="17">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D36" s="20">
-        <v>16693.400000000001</v>
-      </c>
       <c r="E36" s="24">
         <f t="shared" si="4"/>
-        <v>1.3000000000029104</v>
+        <v>-16692.099999999999</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" si="5"/>
-        <v>1.3000000000029104</v>
-      </c>
-      <c r="H36" s="20">
-        <v>16692.900000000001</v>
-      </c>
+        <v>16692.099999999999</v>
+      </c>
+      <c r="H36" s="20"/>
       <c r="I36" s="24">
         <f t="shared" si="6"/>
-        <v>0.80000000000291038</v>
+        <v>-16692.099999999999</v>
       </c>
       <c r="J36" s="10">
         <f t="shared" si="7"/>
-        <v>0.80000000000291038</v>
+        <v>16692.099999999999</v>
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="20">
@@ -3916,28 +3739,24 @@
         <f t="shared" si="9"/>
         <v>1.4000000000014552</v>
       </c>
-      <c r="O36" s="59"/>
-      <c r="P36" s="20">
-        <v>16694.3</v>
-      </c>
+      <c r="O36" s="49"/>
+      <c r="P36" s="20"/>
       <c r="Q36" s="24">
         <f t="shared" si="10"/>
-        <v>2.2000000000007276</v>
+        <v>-16692.099999999999</v>
       </c>
       <c r="R36" s="24">
         <f t="shared" si="11"/>
-        <v>2.2000000000007276</v>
-      </c>
-      <c r="T36" s="20">
-        <v>16701.2</v>
-      </c>
+        <v>16692.099999999999</v>
+      </c>
+      <c r="T36" s="20"/>
       <c r="U36" s="24">
         <f t="shared" si="12"/>
-        <v>9.1000000000021828</v>
+        <v>-16692.099999999999</v>
       </c>
       <c r="V36" s="10">
         <f t="shared" si="13"/>
-        <v>9.1000000000021828</v>
+        <v>16692.099999999999</v>
       </c>
     </row>
     <row r="37" spans="1:22">
@@ -3947,27 +3766,22 @@
       <c r="B37" s="17">
         <v>1.45</v>
       </c>
-      <c r="D37" s="20">
-        <v>16902.8</v>
-      </c>
       <c r="E37" s="24">
         <f t="shared" si="4"/>
-        <v>-0.90000000000145519</v>
+        <v>-16903.7</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" si="5"/>
-        <v>0.90000000000145519</v>
-      </c>
-      <c r="H37" s="20">
-        <v>16902.400000000001</v>
-      </c>
+        <v>16903.7</v>
+      </c>
+      <c r="H37" s="20"/>
       <c r="I37" s="24">
         <f t="shared" si="6"/>
-        <v>-1.2999999999992724</v>
+        <v>-16903.7</v>
       </c>
       <c r="J37" s="10">
         <f t="shared" si="7"/>
-        <v>1.2999999999992724</v>
+        <v>16903.7</v>
       </c>
       <c r="K37" s="10"/>
       <c r="L37" s="20">
@@ -3981,28 +3795,24 @@
         <f t="shared" si="9"/>
         <v>0.60000000000218279</v>
       </c>
-      <c r="O37" s="59"/>
-      <c r="P37" s="20">
-        <v>16904.099999999999</v>
-      </c>
+      <c r="O37" s="49"/>
+      <c r="P37" s="20"/>
       <c r="Q37" s="24">
         <f t="shared" si="10"/>
-        <v>0.39999999999781721</v>
+        <v>-16903.7</v>
       </c>
       <c r="R37" s="24">
         <f t="shared" si="11"/>
-        <v>0.39999999999781721</v>
-      </c>
-      <c r="T37" s="20">
-        <v>16907.5</v>
-      </c>
+        <v>16903.7</v>
+      </c>
+      <c r="T37" s="20"/>
       <c r="U37" s="24">
         <f t="shared" si="12"/>
-        <v>3.7999999999992724</v>
+        <v>-16903.7</v>
       </c>
       <c r="V37" s="10">
         <f t="shared" si="13"/>
-        <v>3.7999999999992724</v>
+        <v>16903.7</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -4012,27 +3822,22 @@
       <c r="B38" s="17">
         <v>1.2</v>
       </c>
-      <c r="D38" s="20">
-        <v>17122.900000000001</v>
-      </c>
       <c r="E38" s="24">
         <f t="shared" si="4"/>
-        <v>-0.69999999999708962</v>
+        <v>-17123.599999999999</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="5"/>
-        <v>0.69999999999708962</v>
-      </c>
-      <c r="H38" s="20">
-        <v>17122.8</v>
-      </c>
+        <v>17123.599999999999</v>
+      </c>
+      <c r="H38" s="20"/>
       <c r="I38" s="24">
         <f t="shared" si="6"/>
-        <v>-0.7999999999992724</v>
+        <v>-17123.599999999999</v>
       </c>
       <c r="J38" s="10">
         <f t="shared" si="7"/>
-        <v>0.7999999999992724</v>
+        <v>17123.599999999999</v>
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="20">
@@ -4046,28 +3851,24 @@
         <f t="shared" si="9"/>
         <v>0.89999999999781721</v>
       </c>
-      <c r="O38" s="59"/>
-      <c r="P38" s="20">
-        <v>17124</v>
-      </c>
+      <c r="O38" s="49"/>
+      <c r="P38" s="20"/>
       <c r="Q38" s="24">
         <f t="shared" si="10"/>
-        <v>0.40000000000145519</v>
+        <v>-17123.599999999999</v>
       </c>
       <c r="R38" s="24">
         <f t="shared" si="11"/>
-        <v>0.40000000000145519</v>
-      </c>
-      <c r="T38" s="20">
-        <v>17126.5</v>
-      </c>
+        <v>17123.599999999999</v>
+      </c>
+      <c r="T38" s="20"/>
       <c r="U38" s="24">
         <f t="shared" si="12"/>
-        <v>2.9000000000014552</v>
+        <v>-17123.599999999999</v>
       </c>
       <c r="V38" s="10">
         <f t="shared" si="13"/>
-        <v>2.9000000000014552</v>
+        <v>17123.599999999999</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -4077,27 +3878,22 @@
       <c r="B39" s="17">
         <v>2</v>
       </c>
-      <c r="D39" s="20">
-        <v>17653.400000000001</v>
-      </c>
       <c r="E39" s="24">
         <f t="shared" si="4"/>
-        <v>0.10000000000218279</v>
+        <v>-17653.3</v>
       </c>
       <c r="F39" s="10">
         <f t="shared" si="5"/>
-        <v>0.10000000000218279</v>
-      </c>
-      <c r="H39" s="20">
-        <v>17653.5</v>
-      </c>
+        <v>17653.3</v>
+      </c>
+      <c r="H39" s="20"/>
       <c r="I39" s="24">
         <f t="shared" si="6"/>
-        <v>0.2000000000007276</v>
+        <v>-17653.3</v>
       </c>
       <c r="J39" s="10">
         <f t="shared" si="7"/>
-        <v>0.2000000000007276</v>
+        <v>17653.3</v>
       </c>
       <c r="K39" s="10"/>
       <c r="L39" s="20">
@@ -4111,28 +3907,24 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="O39" s="59"/>
-      <c r="P39" s="20">
-        <v>17654.8</v>
-      </c>
+      <c r="O39" s="49"/>
+      <c r="P39" s="20"/>
       <c r="Q39" s="24">
         <f t="shared" si="10"/>
-        <v>1.5</v>
+        <v>-17653.3</v>
       </c>
       <c r="R39" s="24">
         <f t="shared" si="11"/>
-        <v>1.5</v>
-      </c>
-      <c r="T39" s="20">
-        <v>17644.400000000001</v>
-      </c>
+        <v>17653.3</v>
+      </c>
+      <c r="T39" s="20"/>
       <c r="U39" s="24">
         <f t="shared" si="12"/>
-        <v>-8.8999999999978172</v>
+        <v>-17653.3</v>
       </c>
       <c r="V39" s="10">
         <f t="shared" si="13"/>
-        <v>8.8999999999978172</v>
+        <v>17653.3</v>
       </c>
     </row>
     <row r="40" spans="1:22">
@@ -4142,27 +3934,22 @@
       <c r="B40" s="17">
         <v>1.2</v>
       </c>
-      <c r="D40" s="20">
-        <v>17879.599999999999</v>
-      </c>
       <c r="E40" s="24">
         <f t="shared" si="4"/>
-        <v>-0.7000000000007276</v>
+        <v>-17880.3</v>
       </c>
       <c r="F40" s="10">
         <f t="shared" si="5"/>
-        <v>0.7000000000007276</v>
-      </c>
-      <c r="H40" s="20">
-        <v>17880</v>
-      </c>
+        <v>17880.3</v>
+      </c>
+      <c r="H40" s="20"/>
       <c r="I40" s="24">
         <f t="shared" si="6"/>
-        <v>-0.2999999999992724</v>
+        <v>-17880.3</v>
       </c>
       <c r="J40" s="10">
         <f t="shared" si="7"/>
-        <v>0.2999999999992724</v>
+        <v>17880.3</v>
       </c>
       <c r="K40" s="10"/>
       <c r="L40" s="20">
@@ -4176,28 +3963,24 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="O40" s="59"/>
-      <c r="P40" s="20">
-        <v>17881.099999999999</v>
-      </c>
+      <c r="O40" s="49"/>
+      <c r="P40" s="20"/>
       <c r="Q40" s="24">
         <f t="shared" si="10"/>
-        <v>0.7999999999992724</v>
+        <v>-17880.3</v>
       </c>
       <c r="R40" s="24">
         <f t="shared" si="11"/>
-        <v>0.7999999999992724</v>
-      </c>
-      <c r="T40" s="20">
-        <v>17882.5</v>
-      </c>
+        <v>17880.3</v>
+      </c>
+      <c r="T40" s="20"/>
       <c r="U40" s="24">
         <f t="shared" si="12"/>
-        <v>2.2000000000007276</v>
+        <v>-17880.3</v>
       </c>
       <c r="V40" s="10">
         <f t="shared" si="13"/>
-        <v>2.2000000000007276</v>
+        <v>17880.3</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -4207,27 +3990,22 @@
       <c r="B41" s="17">
         <v>1.42</v>
       </c>
-      <c r="D41" s="20">
-        <v>17993.400000000001</v>
-      </c>
       <c r="E41" s="24">
         <f t="shared" si="4"/>
-        <v>-0.59999999999854481</v>
+        <v>-17994</v>
       </c>
       <c r="F41" s="10">
         <f t="shared" si="5"/>
-        <v>0.59999999999854481</v>
-      </c>
-      <c r="H41" s="20">
-        <v>17993.7</v>
-      </c>
+        <v>17994</v>
+      </c>
+      <c r="H41" s="20"/>
       <c r="I41" s="24">
         <f t="shared" si="6"/>
-        <v>-0.2999999999992724</v>
+        <v>-17994</v>
       </c>
       <c r="J41" s="10">
         <f t="shared" si="7"/>
-        <v>0.2999999999992724</v>
+        <v>17994</v>
       </c>
       <c r="K41" s="10"/>
       <c r="L41" s="20">
@@ -4241,17 +4019,15 @@
         <f t="shared" si="9"/>
         <v>0.40000000000145519</v>
       </c>
-      <c r="O41" s="59"/>
-      <c r="P41" s="20">
-        <v>17994.8</v>
-      </c>
+      <c r="O41" s="49"/>
+      <c r="P41" s="20"/>
       <c r="Q41" s="24">
         <f t="shared" si="10"/>
-        <v>0.7999999999992724</v>
+        <v>-17994</v>
       </c>
       <c r="R41" s="24">
         <f t="shared" si="11"/>
-        <v>0.7999999999992724</v>
+        <v>17994</v>
       </c>
       <c r="T41" s="20"/>
       <c r="U41" s="24">
@@ -4270,27 +4046,22 @@
       <c r="B42" s="17">
         <v>0.5</v>
       </c>
-      <c r="D42" s="20">
-        <v>18118.7</v>
-      </c>
       <c r="E42" s="24">
         <f t="shared" si="4"/>
-        <v>0.2000000000007276</v>
+        <v>-18118.5</v>
       </c>
       <c r="F42" s="10">
         <f t="shared" si="5"/>
-        <v>0.2000000000007276</v>
-      </c>
-      <c r="H42" s="20">
-        <v>18118.400000000001</v>
-      </c>
+        <v>18118.5</v>
+      </c>
+      <c r="H42" s="20"/>
       <c r="I42" s="24">
         <f t="shared" si="6"/>
-        <v>-9.9999999998544808E-2</v>
+        <v>-18118.5</v>
       </c>
       <c r="J42" s="10">
         <f t="shared" si="7"/>
-        <v>9.9999999998544808E-2</v>
+        <v>18118.5</v>
       </c>
       <c r="K42" s="10"/>
       <c r="L42" s="20">
@@ -4304,17 +4075,15 @@
         <f t="shared" si="9"/>
         <v>9.9999999998544808E-2</v>
       </c>
-      <c r="O42" s="59"/>
-      <c r="P42" s="20">
-        <v>18119.3</v>
-      </c>
+      <c r="O42" s="49"/>
+      <c r="P42" s="20"/>
       <c r="Q42" s="24">
         <f t="shared" si="10"/>
-        <v>0.7999999999992724</v>
+        <v>-18118.5</v>
       </c>
       <c r="R42" s="24">
         <f t="shared" si="11"/>
-        <v>0.7999999999992724</v>
+        <v>18118.5</v>
       </c>
       <c r="T42" s="20"/>
       <c r="U42" s="24">
@@ -4334,7 +4103,7 @@
       <c r="L43" s="20"/>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
-      <c r="O43" s="59"/>
+      <c r="O43" s="49"/>
       <c r="P43" s="20"/>
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
@@ -4349,27 +4118,22 @@
       <c r="B44" s="17">
         <v>0.32</v>
       </c>
-      <c r="D44" s="20">
-        <v>19250.400000000001</v>
-      </c>
       <c r="E44" s="24">
         <f t="shared" ref="E44:E58" si="14">D44-$A44</f>
-        <v>0.10000000000218279</v>
+        <v>-19250.3</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" ref="F44:F58" si="15">ABS(E44)</f>
-        <v>0.10000000000218279</v>
-      </c>
-      <c r="H44" s="20">
-        <v>19250.7</v>
-      </c>
+        <v>19250.3</v>
+      </c>
+      <c r="H44" s="20"/>
       <c r="I44" s="24">
         <f t="shared" ref="I44:I58" si="16">H44-$A44</f>
-        <v>0.40000000000145519</v>
+        <v>-19250.3</v>
       </c>
       <c r="J44" s="10">
         <f t="shared" ref="J44:J58" si="17">ABS(I44)</f>
-        <v>0.40000000000145519</v>
+        <v>19250.3</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="20">
@@ -4383,17 +4147,15 @@
         <f t="shared" ref="N44:N58" si="19">ABS(M44)</f>
         <v>0.2999999999992724</v>
       </c>
-      <c r="O44" s="59"/>
-      <c r="P44" s="20">
-        <v>19251.5</v>
-      </c>
+      <c r="O44" s="49"/>
+      <c r="P44" s="20"/>
       <c r="Q44" s="24">
         <f t="shared" ref="Q44:Q58" si="20">P44-$A44</f>
-        <v>1.2000000000007276</v>
+        <v>-19250.3</v>
       </c>
       <c r="R44" s="24">
         <f t="shared" ref="R44:R58" si="21">ABS(Q44)</f>
-        <v>1.2000000000007276</v>
+        <v>19250.3</v>
       </c>
       <c r="T44" s="20"/>
       <c r="U44" s="24">
@@ -4412,27 +4174,22 @@
       <c r="B45" s="17">
         <v>0.25</v>
       </c>
-      <c r="D45" s="20">
-        <v>19350.5</v>
-      </c>
       <c r="E45" s="24">
         <f t="shared" si="14"/>
-        <v>0.40000000000145519</v>
+        <v>-19350.099999999999</v>
       </c>
       <c r="F45" s="10">
         <f t="shared" si="15"/>
-        <v>0.40000000000145519</v>
-      </c>
-      <c r="H45" s="20">
-        <v>19350.8</v>
-      </c>
+        <v>19350.099999999999</v>
+      </c>
+      <c r="H45" s="20"/>
       <c r="I45" s="24">
         <f t="shared" si="16"/>
-        <v>0.7000000000007276</v>
+        <v>-19350.099999999999</v>
       </c>
       <c r="J45" s="10">
         <f t="shared" si="17"/>
-        <v>0.7000000000007276</v>
+        <v>19350.099999999999</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="20">
@@ -4446,17 +4203,15 @@
         <f t="shared" si="19"/>
         <v>0.2999999999992724</v>
       </c>
-      <c r="O45" s="59"/>
-      <c r="P45" s="20">
-        <v>19351.2</v>
-      </c>
+      <c r="O45" s="49"/>
+      <c r="P45" s="20"/>
       <c r="Q45" s="24">
         <f t="shared" si="20"/>
-        <v>1.1000000000021828</v>
+        <v>-19350.099999999999</v>
       </c>
       <c r="R45" s="24">
         <f t="shared" si="21"/>
-        <v>1.1000000000021828</v>
+        <v>19350.099999999999</v>
       </c>
       <c r="T45" s="20"/>
       <c r="U45" s="24">
@@ -4475,27 +4230,22 @@
       <c r="B46" s="17">
         <v>0.52</v>
       </c>
-      <c r="D46" s="20">
-        <v>19771.099999999999</v>
-      </c>
       <c r="E46" s="24">
         <f t="shared" si="14"/>
-        <v>-0.7000000000007276</v>
+        <v>-19771.8</v>
       </c>
       <c r="F46" s="10">
         <f t="shared" si="15"/>
-        <v>0.7000000000007276</v>
-      </c>
-      <c r="H46" s="20">
-        <v>19772.3</v>
-      </c>
+        <v>19771.8</v>
+      </c>
+      <c r="H46" s="20"/>
       <c r="I46" s="24">
         <f t="shared" si="16"/>
-        <v>0.5</v>
+        <v>-19771.8</v>
       </c>
       <c r="J46" s="10">
         <f t="shared" si="17"/>
-        <v>0.5</v>
+        <v>19771.8</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="20">
@@ -4509,17 +4259,15 @@
         <f t="shared" si="19"/>
         <v>0.59999999999854481</v>
       </c>
-      <c r="O46" s="59"/>
-      <c r="P46" s="20">
-        <v>19772.8</v>
-      </c>
+      <c r="O46" s="49"/>
+      <c r="P46" s="20"/>
       <c r="Q46" s="24">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-19771.8</v>
       </c>
       <c r="R46" s="24">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>19771.8</v>
       </c>
       <c r="T46" s="20"/>
       <c r="U46" s="24">
@@ -4538,27 +4286,22 @@
       <c r="B47" s="17">
         <v>1.05</v>
       </c>
-      <c r="D47" s="20">
-        <v>20008.099999999999</v>
-      </c>
       <c r="E47" s="24">
         <f t="shared" si="14"/>
-        <v>-0.10000000000218279</v>
+        <v>-20008.2</v>
       </c>
       <c r="F47" s="10">
         <f t="shared" si="15"/>
-        <v>0.10000000000218279</v>
-      </c>
-      <c r="H47" s="20">
-        <v>20009.099999999999</v>
-      </c>
+        <v>20008.2</v>
+      </c>
+      <c r="H47" s="20"/>
       <c r="I47" s="24">
         <f t="shared" si="16"/>
-        <v>0.89999999999781721</v>
+        <v>-20008.2</v>
       </c>
       <c r="J47" s="10">
         <f t="shared" si="17"/>
-        <v>0.89999999999781721</v>
+        <v>20008.2</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="20">
@@ -4572,17 +4315,15 @@
         <f t="shared" si="19"/>
         <v>0.2000000000007276</v>
       </c>
-      <c r="O47" s="59"/>
-      <c r="P47" s="20">
-        <v>20009.5</v>
-      </c>
+      <c r="O47" s="49"/>
+      <c r="P47" s="20"/>
       <c r="Q47" s="24">
         <f t="shared" si="20"/>
-        <v>1.2999999999992724</v>
+        <v>-20008.2</v>
       </c>
       <c r="R47" s="24">
         <f t="shared" si="21"/>
-        <v>1.2999999999992724</v>
+        <v>20008.2</v>
       </c>
       <c r="T47" s="20"/>
       <c r="U47" s="24">
@@ -4601,27 +4342,22 @@
       <c r="B48" s="17">
         <v>1</v>
       </c>
-      <c r="D48" s="20">
-        <v>20276.099999999999</v>
-      </c>
       <c r="E48" s="24">
         <f t="shared" si="14"/>
-        <v>0.19999999999708962</v>
+        <v>-20275.900000000001</v>
       </c>
       <c r="F48" s="10">
         <f t="shared" si="15"/>
-        <v>0.19999999999708962</v>
-      </c>
-      <c r="H48" s="20">
-        <v>20277.599999999999</v>
-      </c>
+        <v>20275.900000000001</v>
+      </c>
+      <c r="H48" s="20"/>
       <c r="I48" s="24">
         <f t="shared" si="16"/>
-        <v>1.6999999999970896</v>
+        <v>-20275.900000000001</v>
       </c>
       <c r="J48" s="10">
         <f t="shared" si="17"/>
-        <v>1.6999999999970896</v>
+        <v>20275.900000000001</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="20">
@@ -4635,17 +4371,15 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O48" s="59"/>
-      <c r="P48" s="20">
-        <v>20278.5</v>
-      </c>
+      <c r="O48" s="49"/>
+      <c r="P48" s="20"/>
       <c r="Q48" s="24">
         <f t="shared" si="20"/>
-        <v>2.5999999999985448</v>
+        <v>-20275.900000000001</v>
       </c>
       <c r="R48" s="24">
         <f t="shared" si="21"/>
-        <v>2.5999999999985448</v>
+        <v>20275.900000000001</v>
       </c>
       <c r="T48" s="20"/>
       <c r="U48" s="24">
@@ -4664,27 +4398,22 @@
       <c r="B49" s="17">
         <v>1.28</v>
       </c>
-      <c r="D49" s="20">
-        <v>20412.599999999999</v>
-      </c>
       <c r="E49" s="24">
         <f t="shared" si="14"/>
-        <v>-0.10000000000218279</v>
+        <v>-20412.7</v>
       </c>
       <c r="F49" s="10">
         <f t="shared" si="15"/>
-        <v>0.10000000000218279</v>
-      </c>
-      <c r="H49" s="20">
-        <v>20414.599999999999</v>
-      </c>
+        <v>20412.7</v>
+      </c>
+      <c r="H49" s="20"/>
       <c r="I49" s="24">
         <f t="shared" si="16"/>
-        <v>1.8999999999978172</v>
+        <v>-20412.7</v>
       </c>
       <c r="J49" s="10">
         <f t="shared" si="17"/>
-        <v>1.8999999999978172</v>
+        <v>20412.7</v>
       </c>
       <c r="K49" s="10"/>
       <c r="L49" s="20">
@@ -4698,17 +4427,15 @@
         <f t="shared" si="19"/>
         <v>0.10000000000218279</v>
       </c>
-      <c r="O49" s="59"/>
-      <c r="P49" s="20">
-        <v>20415.2</v>
-      </c>
+      <c r="O49" s="49"/>
+      <c r="P49" s="20"/>
       <c r="Q49" s="24">
         <f t="shared" si="20"/>
-        <v>2.5</v>
+        <v>-20412.7</v>
       </c>
       <c r="R49" s="24">
         <f t="shared" si="21"/>
-        <v>2.5</v>
+        <v>20412.7</v>
       </c>
       <c r="T49" s="20"/>
       <c r="U49" s="24">
@@ -4727,27 +4454,22 @@
       <c r="B50" s="17">
         <v>1.05</v>
       </c>
-      <c r="D50" s="20">
-        <v>20563.5</v>
-      </c>
       <c r="E50" s="24">
         <f t="shared" si="14"/>
-        <v>-9.9999999998544808E-2</v>
+        <v>-20563.599999999999</v>
       </c>
       <c r="F50" s="10">
         <f t="shared" si="15"/>
-        <v>9.9999999998544808E-2</v>
-      </c>
-      <c r="H50" s="20">
-        <v>20565.8</v>
-      </c>
+        <v>20563.599999999999</v>
+      </c>
+      <c r="H50" s="20"/>
       <c r="I50" s="24">
         <f t="shared" si="16"/>
-        <v>2.2000000000007276</v>
+        <v>-20563.599999999999</v>
       </c>
       <c r="J50" s="10">
         <f t="shared" si="17"/>
-        <v>2.2000000000007276</v>
+        <v>20563.599999999999</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="20">
@@ -4761,17 +4483,15 @@
         <f t="shared" si="19"/>
         <v>0.30000000000291038</v>
       </c>
-      <c r="O50" s="59"/>
-      <c r="P50" s="20">
-        <v>20566.3</v>
-      </c>
+      <c r="O50" s="49"/>
+      <c r="P50" s="20"/>
       <c r="Q50" s="24">
         <f t="shared" si="20"/>
-        <v>2.7000000000007276</v>
+        <v>-20563.599999999999</v>
       </c>
       <c r="R50" s="24">
         <f t="shared" si="21"/>
-        <v>2.7000000000007276</v>
+        <v>20563.599999999999</v>
       </c>
       <c r="T50" s="20"/>
       <c r="U50" s="24">
@@ -4790,27 +4510,22 @@
       <c r="B51" s="17">
         <v>0.77</v>
       </c>
-      <c r="D51" s="20">
-        <v>20729.2</v>
-      </c>
       <c r="E51" s="24">
         <f t="shared" si="14"/>
-        <v>0.2000000000007276</v>
+        <v>-20729</v>
       </c>
       <c r="F51" s="10">
         <f t="shared" si="15"/>
-        <v>0.2000000000007276</v>
-      </c>
-      <c r="H51" s="20">
-        <v>20731.7</v>
-      </c>
+        <v>20729</v>
+      </c>
+      <c r="H51" s="20"/>
       <c r="I51" s="24">
         <f t="shared" si="16"/>
-        <v>2.7000000000007276</v>
+        <v>-20729</v>
       </c>
       <c r="J51" s="10">
         <f t="shared" si="17"/>
-        <v>2.7000000000007276</v>
+        <v>20729</v>
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="20">
@@ -4824,17 +4539,15 @@
         <f t="shared" si="19"/>
         <v>0.7000000000007276</v>
       </c>
-      <c r="O51" s="59"/>
-      <c r="P51" s="20">
-        <v>20732.2</v>
-      </c>
+      <c r="O51" s="49"/>
+      <c r="P51" s="20"/>
       <c r="Q51" s="24">
         <f t="shared" si="20"/>
-        <v>3.2000000000007276</v>
+        <v>-20729</v>
       </c>
       <c r="R51" s="24">
         <f t="shared" si="21"/>
-        <v>3.2000000000007276</v>
+        <v>20729</v>
       </c>
       <c r="T51" s="20"/>
       <c r="U51" s="24">
@@ -4853,27 +4566,22 @@
       <c r="B52" s="17">
         <v>0.38</v>
       </c>
-      <c r="D52" s="20">
-        <v>21176</v>
-      </c>
       <c r="E52" s="24">
         <f t="shared" si="14"/>
-        <v>-0.59999999999854481</v>
+        <v>-21176.6</v>
       </c>
       <c r="F52" s="10">
         <f t="shared" si="15"/>
-        <v>0.59999999999854481</v>
-      </c>
-      <c r="H52" s="20">
-        <v>21179.7</v>
-      </c>
+        <v>21176.6</v>
+      </c>
+      <c r="H52" s="20"/>
       <c r="I52" s="24">
         <f t="shared" si="16"/>
-        <v>3.1000000000021828</v>
+        <v>-21176.6</v>
       </c>
       <c r="J52" s="10">
         <f t="shared" si="17"/>
-        <v>3.1000000000021828</v>
+        <v>21176.6</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="20">
@@ -4887,17 +4595,15 @@
         <f t="shared" si="19"/>
         <v>0.80000000000291038</v>
       </c>
-      <c r="O52" s="59"/>
-      <c r="P52" s="20">
-        <v>21180.400000000001</v>
-      </c>
+      <c r="O52" s="49"/>
+      <c r="P52" s="20"/>
       <c r="Q52" s="24">
         <f t="shared" si="20"/>
-        <v>3.8000000000029104</v>
+        <v>-21176.6</v>
       </c>
       <c r="R52" s="24">
         <f t="shared" si="21"/>
-        <v>3.8000000000029104</v>
+        <v>21176.6</v>
       </c>
       <c r="T52" s="20"/>
       <c r="U52" s="24">
@@ -4916,27 +4622,22 @@
       <c r="B53" s="17">
         <v>0.41</v>
       </c>
-      <c r="D53" s="20">
-        <v>21247.5</v>
-      </c>
       <c r="E53" s="24">
         <f t="shared" si="14"/>
-        <v>-2.2000000000007276</v>
+        <v>-21249.7</v>
       </c>
       <c r="F53" s="10">
         <f t="shared" si="15"/>
-        <v>2.2000000000007276</v>
-      </c>
-      <c r="H53" s="20">
-        <v>21250.2</v>
-      </c>
+        <v>21249.7</v>
+      </c>
+      <c r="H53" s="20"/>
       <c r="I53" s="24">
         <f t="shared" si="16"/>
-        <v>0.5</v>
+        <v>-21249.7</v>
       </c>
       <c r="J53" s="10">
         <f t="shared" si="17"/>
-        <v>0.5</v>
+        <v>21249.7</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="20">
@@ -4950,17 +4651,15 @@
         <f t="shared" si="19"/>
         <v>2.7000000000007276</v>
       </c>
-      <c r="O53" s="59"/>
-      <c r="P53" s="20">
-        <v>21250.6</v>
-      </c>
+      <c r="O53" s="49"/>
+      <c r="P53" s="20"/>
       <c r="Q53" s="24">
         <f t="shared" si="20"/>
-        <v>0.89999999999781721</v>
+        <v>-21249.7</v>
       </c>
       <c r="R53" s="24">
         <f t="shared" si="21"/>
-        <v>0.89999999999781721</v>
+        <v>21249.7</v>
       </c>
       <c r="T53" s="20"/>
       <c r="U53" s="24">
@@ -4979,27 +4678,22 @@
       <c r="B54" s="17">
         <v>1.2</v>
       </c>
-      <c r="D54" s="20">
-        <v>21507.200000000001</v>
-      </c>
       <c r="E54" s="24">
         <f t="shared" si="14"/>
-        <v>-9.9999999998544808E-2</v>
+        <v>-21507.3</v>
       </c>
       <c r="F54" s="10">
         <f t="shared" si="15"/>
-        <v>9.9999999998544808E-2</v>
-      </c>
-      <c r="H54" s="20">
-        <v>21510.799999999999</v>
-      </c>
+        <v>21507.3</v>
+      </c>
+      <c r="H54" s="20"/>
       <c r="I54" s="24">
         <f t="shared" si="16"/>
-        <v>3.5</v>
+        <v>-21507.3</v>
       </c>
       <c r="J54" s="10">
         <f t="shared" si="17"/>
-        <v>3.5</v>
+        <v>21507.3</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="20">
@@ -5013,17 +4707,15 @@
         <f t="shared" si="19"/>
         <v>0.2000000000007276</v>
       </c>
-      <c r="O54" s="59"/>
-      <c r="P54" s="20">
-        <v>21511</v>
-      </c>
+      <c r="O54" s="49"/>
+      <c r="P54" s="20"/>
       <c r="Q54" s="24">
         <f t="shared" si="20"/>
-        <v>3.7000000000007276</v>
+        <v>-21507.3</v>
       </c>
       <c r="R54" s="24">
         <f t="shared" si="21"/>
-        <v>3.7000000000007276</v>
+        <v>21507.3</v>
       </c>
       <c r="T54" s="20"/>
       <c r="U54" s="24">
@@ -5042,27 +4734,22 @@
       <c r="B55" s="17">
         <v>0.7</v>
       </c>
-      <c r="D55" s="20">
-        <v>21802</v>
-      </c>
       <c r="E55" s="24">
         <f t="shared" si="14"/>
-        <v>-0.2000000000007276</v>
+        <v>-21802.2</v>
       </c>
       <c r="F55" s="10">
         <f t="shared" si="15"/>
-        <v>0.2000000000007276</v>
-      </c>
-      <c r="H55" s="20">
-        <v>21806</v>
-      </c>
+        <v>21802.2</v>
+      </c>
+      <c r="H55" s="20"/>
       <c r="I55" s="24">
         <f t="shared" si="16"/>
-        <v>3.7999999999992724</v>
+        <v>-21802.2</v>
       </c>
       <c r="J55" s="10">
         <f t="shared" si="17"/>
-        <v>3.7999999999992724</v>
+        <v>21802.2</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="20">
@@ -5076,17 +4763,15 @@
         <f t="shared" si="19"/>
         <v>0.89999999999781721</v>
       </c>
-      <c r="O55" s="59"/>
-      <c r="P55" s="20">
-        <v>21806.3</v>
-      </c>
+      <c r="O55" s="49"/>
+      <c r="P55" s="20"/>
       <c r="Q55" s="24">
         <f t="shared" si="20"/>
-        <v>4.0999999999985448</v>
+        <v>-21802.2</v>
       </c>
       <c r="R55" s="24">
         <f t="shared" si="21"/>
-        <v>4.0999999999985448</v>
+        <v>21802.2</v>
       </c>
       <c r="T55" s="20"/>
       <c r="U55" s="24">
@@ -5105,27 +4790,22 @@
       <c r="B56" s="17">
         <v>0.9</v>
       </c>
-      <c r="D56" s="20">
-        <v>21956.6</v>
-      </c>
       <c r="E56" s="24">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-21955.599999999999</v>
       </c>
       <c r="F56" s="10">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="H56" s="20">
-        <v>21959.3</v>
-      </c>
+        <v>21955.599999999999</v>
+      </c>
+      <c r="H56" s="20"/>
       <c r="I56" s="24">
         <f t="shared" si="16"/>
-        <v>3.7000000000007276</v>
+        <v>-21955.599999999999</v>
       </c>
       <c r="J56" s="10">
         <f t="shared" si="17"/>
-        <v>3.7000000000007276</v>
+        <v>21955.599999999999</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="20">
@@ -5139,17 +4819,15 @@
         <f t="shared" si="19"/>
         <v>0.7000000000007276</v>
       </c>
-      <c r="O56" s="59"/>
-      <c r="P56" s="20">
-        <v>21959.5</v>
-      </c>
+      <c r="O56" s="49"/>
+      <c r="P56" s="20"/>
       <c r="Q56" s="24">
         <f t="shared" si="20"/>
-        <v>3.9000000000014552</v>
+        <v>-21955.599999999999</v>
       </c>
       <c r="R56" s="24">
         <f t="shared" si="21"/>
-        <v>3.9000000000014552</v>
+        <v>21955.599999999999</v>
       </c>
       <c r="T56" s="20"/>
       <c r="U56" s="24">
@@ -5168,27 +4846,22 @@
       <c r="B57" s="17">
         <v>0.8</v>
       </c>
-      <c r="D57" s="20">
-        <v>22126.9</v>
-      </c>
       <c r="E57" s="24">
         <f t="shared" si="14"/>
-        <v>1.4000000000014552</v>
+        <v>-22125.5</v>
       </c>
       <c r="F57" s="10">
         <f t="shared" si="15"/>
-        <v>1.4000000000014552</v>
-      </c>
-      <c r="H57" s="20">
-        <v>22130.5</v>
-      </c>
+        <v>22125.5</v>
+      </c>
+      <c r="H57" s="20"/>
       <c r="I57" s="24">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>-22125.5</v>
       </c>
       <c r="J57" s="10">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>22125.5</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="20">
@@ -5202,17 +4875,15 @@
         <f t="shared" si="19"/>
         <v>0.59999999999854481</v>
       </c>
-      <c r="O57" s="59"/>
-      <c r="P57" s="20">
-        <v>22130.400000000001</v>
-      </c>
+      <c r="O57" s="49"/>
+      <c r="P57" s="20"/>
       <c r="Q57" s="24">
         <f t="shared" si="20"/>
-        <v>4.9000000000014552</v>
+        <v>-22125.5</v>
       </c>
       <c r="R57" s="24">
         <f t="shared" si="21"/>
-        <v>4.9000000000014552</v>
+        <v>22125.5</v>
       </c>
       <c r="T57" s="20"/>
       <c r="U57" s="24">
@@ -5231,27 +4902,22 @@
       <c r="B58" s="17">
         <v>0.5</v>
       </c>
-      <c r="D58" s="20">
-        <v>22315.8</v>
-      </c>
       <c r="E58" s="24">
         <f t="shared" si="14"/>
-        <v>3.0999999999985448</v>
+        <v>-22312.7</v>
       </c>
       <c r="F58" s="10">
         <f t="shared" si="15"/>
-        <v>3.0999999999985448</v>
-      </c>
-      <c r="H58" s="20">
-        <v>22319.7</v>
-      </c>
+        <v>22312.7</v>
+      </c>
+      <c r="H58" s="20"/>
       <c r="I58" s="24">
         <f t="shared" si="16"/>
-        <v>7</v>
+        <v>-22312.7</v>
       </c>
       <c r="J58" s="10">
         <f t="shared" si="17"/>
-        <v>7</v>
+        <v>22312.7</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="20">
@@ -5265,17 +4931,15 @@
         <f t="shared" si="19"/>
         <v>2.2000000000007276</v>
       </c>
-      <c r="O58" s="59"/>
-      <c r="P58" s="20">
-        <v>22319.8</v>
-      </c>
+      <c r="O58" s="49"/>
+      <c r="P58" s="20"/>
       <c r="Q58" s="24">
         <f t="shared" si="20"/>
-        <v>7.0999999999985448</v>
+        <v>-22312.7</v>
       </c>
       <c r="R58" s="24">
         <f t="shared" si="21"/>
-        <v>7.0999999999985448</v>
+        <v>22312.7</v>
       </c>
       <c r="T58" s="20"/>
       <c r="U58" s="24">
@@ -5295,7 +4959,7 @@
       <c r="L59" s="20"/>
       <c r="M59" s="24"/>
       <c r="N59" s="24"/>
-      <c r="O59" s="59"/>
+      <c r="O59" s="49"/>
       <c r="P59" s="20"/>
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
@@ -5311,7 +4975,7 @@
       <c r="L60" s="20"/>
       <c r="M60" s="24"/>
       <c r="N60" s="24"/>
-      <c r="O60" s="59"/>
+      <c r="O60" s="49"/>
       <c r="P60" s="20"/>
       <c r="Q60" s="24"/>
       <c r="R60" s="24"/>
@@ -5325,22 +4989,22 @@
       </c>
       <c r="E61" s="24">
         <f>AVERAGE(E27:E42,E44:E58)</f>
-        <v>-0.29677419354817586</v>
+        <v>-18574.216129032258</v>
       </c>
       <c r="F61" s="10">
         <f>AVERAGE(F27:F42,F44:F58)</f>
-        <v>0.81290322580670982</v>
+        <v>18574.216129032258</v>
       </c>
       <c r="H61" s="20" t="s">
         <v>67</v>
       </c>
       <c r="I61" s="24">
         <f>AVERAGE(I27:I42,I44:I58)</f>
-        <v>0.6419354838711907</v>
+        <v>-18574.216129032258</v>
       </c>
       <c r="J61" s="10">
         <f>AVERAGE(J27:J42,J44:J58)</f>
-        <v>1.8483870967741114</v>
+        <v>18574.216129032258</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="20" t="s">
@@ -5354,28 +5018,28 @@
         <f>AVERAGE(N27:N42,N44:N58)</f>
         <v>0.79032258064533734</v>
       </c>
-      <c r="O61" s="59"/>
+      <c r="O61" s="49"/>
       <c r="P61" s="20" t="s">
         <v>67</v>
       </c>
       <c r="Q61" s="24">
         <f>AVERAGE(Q27:Q42,Q44:Q58)</f>
-        <v>1.5935483870968798</v>
+        <v>-18574.216129032258</v>
       </c>
       <c r="R61" s="24">
         <f>AVERAGE(R27:R42,R44:R58)</f>
-        <v>1.8064516129031671</v>
+        <v>18574.216129032258</v>
       </c>
       <c r="T61" s="20" t="s">
         <v>67</v>
       </c>
       <c r="U61" s="24">
         <f>AVERAGE(U4:U40)</f>
-        <v>1.3857142857144416</v>
+        <v>-14299.385714285712</v>
       </c>
       <c r="V61" s="10">
         <f>AVERAGE(V4:V40)</f>
-        <v>2.6485714285715014</v>
+        <v>14299.385714285712</v>
       </c>
     </row>
     <row r="62" spans="1:22">
@@ -5384,22 +5048,22 @@
       </c>
       <c r="E62" s="24">
         <f>STDEV(E27:E42,E44:E58)</f>
-        <v>1.1145952541821846</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="F62" s="10">
         <f>STDEV(F27:F42,F44:F58)</f>
-        <v>0.80653246906472276</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="H62" s="20" t="s">
         <v>68</v>
       </c>
       <c r="I62" s="24">
         <f>STDEV(I27:I42,I44:I58)</f>
-        <v>2.3548211812574138</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="J62" s="10">
         <f>STDEV(J27:J42,J44:J58)</f>
-        <v>1.5622357841124808</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="20" t="s">
@@ -5413,28 +5077,28 @@
         <f>STDEV(N27:N42,N44:N58)</f>
         <v>0.74132981356023664</v>
       </c>
-      <c r="O62" s="59"/>
+      <c r="O62" s="49"/>
       <c r="P62" s="20" t="s">
         <v>68</v>
       </c>
       <c r="Q62" s="24">
         <f>STDEV(Q27:Q42,Q44:Q58)</f>
-        <v>1.8741994706845406</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="R62" s="24">
         <f>STDEV(R27:R42,R44:R58)</f>
-        <v>1.662715747178326</v>
+        <v>2439.5452375524228</v>
       </c>
       <c r="T62" s="20" t="s">
         <v>68</v>
       </c>
       <c r="U62" s="24">
         <f>STDEV(U4:U40)</f>
-        <v>3.6470893194712271</v>
+        <v>2022.2305628923277</v>
       </c>
       <c r="V62" s="10">
         <f>STDEV(V4:V40)</f>
-        <v>2.8384307417356021</v>
+        <v>2022.2305628923277</v>
       </c>
     </row>
     <row r="67" spans="8:12">
@@ -5658,8 +5322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5672,23 +5336,23 @@
   <sheetData>
     <row r="1" spans="1:13" s="23" customFormat="1">
       <c r="A1" s="22"/>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="26"/>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="46"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="53"/>
       <c r="J1" s="27"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="58"/>
     </row>
     <row r="2" spans="1:13" s="11" customFormat="1" ht="46" thickBot="1">
       <c r="A2" s="13" t="s">
@@ -6056,27 +5720,23 @@
       <c r="A14" s="5">
         <v>13370.8</v>
       </c>
-      <c r="C14" s="20">
-        <v>13369.2</v>
-      </c>
+      <c r="C14" s="20"/>
       <c r="D14" s="24">
         <f t="shared" ref="D14:D24" si="6">C14-$A14</f>
-        <v>-1.5999999999985448</v>
+        <v>-13370.8</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" ref="E14:E24" si="7">ABS(D14)</f>
-        <v>1.5999999999985448</v>
-      </c>
-      <c r="G14" s="25">
-        <v>13370</v>
-      </c>
+        <v>13370.8</v>
+      </c>
+      <c r="G14" s="25"/>
       <c r="H14" s="24">
         <f t="shared" ref="H14:H24" si="8">G14-$A14</f>
-        <v>-0.7999999999992724</v>
+        <v>-13370.8</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" ref="I14:I24" si="9">ABS(H14)</f>
-        <v>0.7999999999992724</v>
+        <v>13370.8</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="24">
@@ -6092,27 +5752,23 @@
       <c r="A15" s="5">
         <v>13507.9</v>
       </c>
-      <c r="C15" s="20">
-        <v>13506.7</v>
-      </c>
+      <c r="C15" s="20"/>
       <c r="D15" s="24">
         <f t="shared" si="6"/>
-        <v>-1.1999999999989086</v>
+        <v>-13507.9</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="7"/>
-        <v>1.1999999999989086</v>
-      </c>
-      <c r="G15" s="25">
-        <v>13505.4</v>
-      </c>
+        <v>13507.9</v>
+      </c>
+      <c r="G15" s="25"/>
       <c r="H15" s="24">
         <f t="shared" si="8"/>
-        <v>-2.5</v>
+        <v>-13507.9</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" si="9"/>
-        <v>2.5</v>
+        <v>13507.9</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="24">
@@ -6128,27 +5784,23 @@
       <c r="A16" s="5">
         <v>13722.3</v>
       </c>
-      <c r="C16" s="20">
-        <v>13721.4</v>
-      </c>
+      <c r="C16" s="20"/>
       <c r="D16" s="24">
         <f t="shared" si="6"/>
-        <v>-0.8999999999996362</v>
+        <v>-13722.3</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="7"/>
-        <v>0.8999999999996362</v>
-      </c>
-      <c r="G16" s="25">
-        <v>13721.5</v>
-      </c>
+        <v>13722.3</v>
+      </c>
+      <c r="G16" s="25"/>
       <c r="H16" s="24">
         <f t="shared" si="8"/>
-        <v>-0.7999999999992724</v>
+        <v>-13722.3</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="9"/>
-        <v>0.7999999999992724</v>
+        <v>13722.3</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="24">
@@ -6164,27 +5816,23 @@
       <c r="A17" s="5">
         <v>14097.5</v>
       </c>
-      <c r="C17" s="20">
-        <v>14095.7</v>
-      </c>
+      <c r="C17" s="20"/>
       <c r="D17" s="24">
         <f t="shared" si="6"/>
-        <v>-1.7999999999992724</v>
+        <v>-14097.5</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="7"/>
-        <v>1.7999999999992724</v>
-      </c>
-      <c r="G17" s="54">
-        <v>14095.6</v>
-      </c>
+        <v>14097.5</v>
+      </c>
+      <c r="G17" s="44"/>
       <c r="H17" s="24">
         <f t="shared" si="8"/>
-        <v>-1.8999999999996362</v>
+        <v>-14097.5</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="9"/>
-        <v>1.8999999999996362</v>
+        <v>14097.5</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="24">
@@ -6200,27 +5848,23 @@
       <c r="A18" s="5">
         <v>15050.6</v>
       </c>
-      <c r="C18" s="20">
-        <v>15048.6</v>
-      </c>
+      <c r="C18" s="20"/>
       <c r="D18" s="24">
         <f t="shared" si="6"/>
-        <v>-2</v>
+        <v>-15050.6</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="G18" s="54">
-        <v>15048.4</v>
-      </c>
+        <v>15050.6</v>
+      </c>
+      <c r="G18" s="44"/>
       <c r="H18" s="24">
         <f t="shared" si="8"/>
-        <v>-2.2000000000007276</v>
+        <v>-15050.6</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="9"/>
-        <v>2.2000000000007276</v>
+        <v>15050.6</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="24">
@@ -6236,27 +5880,23 @@
       <c r="A19" s="5">
         <v>15993.9</v>
       </c>
-      <c r="C19" s="20">
-        <v>15993.3</v>
-      </c>
+      <c r="C19" s="20"/>
       <c r="D19" s="24">
         <f t="shared" si="6"/>
-        <v>-0.6000000000003638</v>
+        <v>-15993.9</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="7"/>
-        <v>0.6000000000003638</v>
-      </c>
-      <c r="G19" s="54">
-        <v>15993.5</v>
-      </c>
+        <v>15993.9</v>
+      </c>
+      <c r="G19" s="44"/>
       <c r="H19" s="24">
         <f t="shared" si="8"/>
-        <v>-0.3999999999996362</v>
+        <v>-15993.9</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" si="9"/>
-        <v>0.3999999999996362</v>
+        <v>15993.9</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="24">
@@ -6272,27 +5912,23 @@
       <c r="A20" s="5">
         <v>16524.400000000001</v>
       </c>
-      <c r="C20" s="20">
-        <v>16524.2</v>
-      </c>
+      <c r="C20" s="20"/>
       <c r="D20" s="24">
         <f t="shared" si="6"/>
-        <v>-0.2000000000007276</v>
+        <v>-16524.400000000001</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="7"/>
-        <v>0.2000000000007276</v>
-      </c>
-      <c r="G20" s="54">
-        <v>16524</v>
-      </c>
+        <v>16524.400000000001</v>
+      </c>
+      <c r="G20" s="44"/>
       <c r="H20" s="24">
         <f t="shared" si="8"/>
-        <v>-0.40000000000145519</v>
+        <v>-16524.400000000001</v>
       </c>
       <c r="I20" s="9">
         <f t="shared" si="9"/>
-        <v>0.40000000000145519</v>
+        <v>16524.400000000001</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="24">
@@ -6308,27 +5944,23 @@
       <c r="A21" s="5">
         <v>16744.7</v>
       </c>
-      <c r="C21" s="20">
-        <v>16745.2</v>
-      </c>
+      <c r="C21" s="20"/>
       <c r="D21" s="24">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>-16744.7</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="54">
-        <v>16744.599999999999</v>
-      </c>
+        <v>16744.7</v>
+      </c>
+      <c r="G21" s="44"/>
       <c r="H21" s="24">
         <f t="shared" si="8"/>
-        <v>-0.10000000000218279</v>
+        <v>-16744.7</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" si="9"/>
-        <v>0.10000000000218279</v>
+        <v>16744.7</v>
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="24">
@@ -6344,27 +5976,23 @@
       <c r="A22" s="5">
         <v>16945.2</v>
       </c>
-      <c r="C22" s="20">
-        <v>16944.599999999999</v>
-      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="24">
         <f t="shared" si="6"/>
-        <v>-0.60000000000218279</v>
+        <v>-16945.2</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="7"/>
-        <v>0.60000000000218279</v>
-      </c>
-      <c r="G22" s="54">
-        <v>16944.2</v>
-      </c>
+        <v>16945.2</v>
+      </c>
+      <c r="G22" s="44"/>
       <c r="H22" s="24">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>-16945.2</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>16945.2</v>
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="24">
@@ -6380,27 +6008,23 @@
       <c r="A23" s="5">
         <v>17449.8</v>
       </c>
-      <c r="C23" s="20">
-        <v>17450.8</v>
-      </c>
+      <c r="C23" s="20"/>
       <c r="D23" s="24">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-17449.8</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G23" s="54">
-        <v>17450.5</v>
-      </c>
+        <v>17449.8</v>
+      </c>
+      <c r="G23" s="44"/>
       <c r="H23" s="24">
         <f t="shared" si="8"/>
-        <v>0.7000000000007276</v>
+        <v>-17449.8</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="9"/>
-        <v>0.7000000000007276</v>
+        <v>17449.8</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="24">
@@ -6416,27 +6040,23 @@
       <c r="A24" s="5">
         <v>17919.599999999999</v>
       </c>
-      <c r="C24" s="20">
-        <v>17916.3</v>
-      </c>
+      <c r="C24" s="20"/>
       <c r="D24" s="24">
         <f t="shared" si="6"/>
-        <v>-3.2999999999992724</v>
+        <v>-17919.599999999999</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="7"/>
-        <v>3.2999999999992724</v>
-      </c>
-      <c r="G24" s="54">
-        <v>17919.8</v>
-      </c>
+        <v>17919.599999999999</v>
+      </c>
+      <c r="G24" s="44"/>
       <c r="H24" s="24">
         <f t="shared" si="8"/>
-        <v>0.2000000000007276</v>
+        <v>-17919.599999999999</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="9"/>
-        <v>0.2000000000007276</v>
+        <v>17919.599999999999</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="24">
@@ -6463,27 +6083,23 @@
       <c r="A26" s="5">
         <v>18432.8</v>
       </c>
-      <c r="C26" s="20">
-        <v>18433.2</v>
-      </c>
+      <c r="C26" s="20"/>
       <c r="D26" s="24">
         <f t="shared" ref="D26:D37" si="12">C26-$A26</f>
-        <v>0.40000000000145519</v>
+        <v>-18432.8</v>
       </c>
       <c r="E26" s="9">
         <f t="shared" ref="E26:E37" si="13">ABS(D26)</f>
-        <v>0.40000000000145519</v>
-      </c>
-      <c r="G26" s="54">
-        <v>18433.400000000001</v>
-      </c>
+        <v>18432.8</v>
+      </c>
+      <c r="G26" s="44"/>
       <c r="H26" s="24">
         <f t="shared" ref="H26:H37" si="14">G26-$A26</f>
-        <v>0.60000000000218279</v>
+        <v>-18432.8</v>
       </c>
       <c r="I26" s="9">
         <f t="shared" ref="I26:I37" si="15">ABS(H26)</f>
-        <v>0.60000000000218279</v>
+        <v>18432.8</v>
       </c>
       <c r="K26" s="7"/>
       <c r="L26" s="24">
@@ -6499,27 +6115,23 @@
       <c r="A27" s="5">
         <v>19822.900000000001</v>
       </c>
-      <c r="C27" s="20">
-        <v>19823.8</v>
-      </c>
+      <c r="C27" s="20"/>
       <c r="D27" s="24">
         <f t="shared" si="12"/>
-        <v>0.89999999999781721</v>
+        <v>-19822.900000000001</v>
       </c>
       <c r="E27" s="9">
         <f t="shared" si="13"/>
-        <v>0.89999999999781721</v>
-      </c>
-      <c r="G27" s="54">
-        <v>19823.2</v>
-      </c>
+        <v>19822.900000000001</v>
+      </c>
+      <c r="G27" s="44"/>
       <c r="H27" s="24">
         <f t="shared" si="14"/>
-        <v>0.2999999999992724</v>
+        <v>-19822.900000000001</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" si="15"/>
-        <v>0.2999999999992724</v>
+        <v>19822.900000000001</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="24">
@@ -6535,27 +6147,23 @@
       <c r="A28" s="5">
         <v>19971.2</v>
       </c>
-      <c r="C28" s="20">
-        <v>19970.400000000001</v>
-      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="24">
         <f t="shared" si="12"/>
-        <v>-0.7999999999992724</v>
+        <v>-19971.2</v>
       </c>
       <c r="E28" s="9">
         <f t="shared" si="13"/>
-        <v>0.7999999999992724</v>
-      </c>
-      <c r="G28" s="54">
-        <v>19970.900000000001</v>
-      </c>
+        <v>19971.2</v>
+      </c>
+      <c r="G28" s="44"/>
       <c r="H28" s="24">
         <f t="shared" si="14"/>
-        <v>-0.2999999999992724</v>
+        <v>-19971.2</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="15"/>
-        <v>0.2999999999992724</v>
+        <v>19971.2</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="24">
@@ -6571,27 +6179,23 @@
       <c r="A29" s="5">
         <v>20322.599999999999</v>
       </c>
-      <c r="C29" s="20">
-        <v>20321.7</v>
-      </c>
+      <c r="C29" s="20"/>
       <c r="D29" s="24">
         <f t="shared" si="12"/>
-        <v>-0.89999999999781721</v>
+        <v>-20322.599999999999</v>
       </c>
       <c r="E29" s="9">
         <f t="shared" si="13"/>
-        <v>0.89999999999781721</v>
-      </c>
-      <c r="G29" s="54">
-        <v>20322.900000000001</v>
-      </c>
+        <v>20322.599999999999</v>
+      </c>
+      <c r="G29" s="44"/>
       <c r="H29" s="24">
         <f t="shared" si="14"/>
-        <v>0.30000000000291038</v>
+        <v>-20322.599999999999</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="15"/>
-        <v>0.30000000000291038</v>
+        <v>20322.599999999999</v>
       </c>
       <c r="K29" s="7"/>
       <c r="L29" s="24">
@@ -6607,27 +6211,23 @@
       <c r="A30" s="5">
         <v>20621.900000000001</v>
       </c>
-      <c r="C30" s="20">
-        <v>20622.2</v>
-      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="24">
         <f t="shared" si="12"/>
-        <v>0.2999999999992724</v>
+        <v>-20621.900000000001</v>
       </c>
       <c r="E30" s="9">
         <f t="shared" si="13"/>
-        <v>0.2999999999992724</v>
-      </c>
-      <c r="G30" s="54">
-        <v>20621.5</v>
-      </c>
+        <v>20621.900000000001</v>
+      </c>
+      <c r="G30" s="44"/>
       <c r="H30" s="24">
         <f t="shared" si="14"/>
-        <v>-0.40000000000145519</v>
+        <v>-20621.900000000001</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="15"/>
-        <v>0.40000000000145519</v>
+        <v>20621.900000000001</v>
       </c>
       <c r="K30" s="7"/>
       <c r="L30" s="24">
@@ -6643,27 +6243,23 @@
       <c r="A31" s="5">
         <v>20991.8</v>
       </c>
-      <c r="C31" s="20">
-        <v>20991.1</v>
-      </c>
+      <c r="C31" s="20"/>
       <c r="D31" s="24">
         <f t="shared" si="12"/>
-        <v>-0.7000000000007276</v>
+        <v>-20991.8</v>
       </c>
       <c r="E31" s="9">
         <f t="shared" si="13"/>
-        <v>0.7000000000007276</v>
-      </c>
-      <c r="G31" s="54">
-        <v>20992.400000000001</v>
-      </c>
+        <v>20991.8</v>
+      </c>
+      <c r="G31" s="44"/>
       <c r="H31" s="24">
         <f t="shared" si="14"/>
-        <v>0.60000000000218279</v>
+        <v>-20991.8</v>
       </c>
       <c r="I31" s="9">
         <f t="shared" si="15"/>
-        <v>0.60000000000218279</v>
+        <v>20991.8</v>
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="24">
@@ -6679,27 +6275,23 @@
       <c r="A32" s="5">
         <v>21338.7</v>
       </c>
-      <c r="C32" s="20">
-        <v>21338.400000000001</v>
-      </c>
+      <c r="C32" s="20"/>
       <c r="D32" s="24">
         <f t="shared" si="12"/>
-        <v>-0.2999999999992724</v>
+        <v>-21338.7</v>
       </c>
       <c r="E32" s="9">
         <f t="shared" si="13"/>
-        <v>0.2999999999992724</v>
-      </c>
-      <c r="G32" s="54">
-        <v>21339.200000000001</v>
-      </c>
+        <v>21338.7</v>
+      </c>
+      <c r="G32" s="44"/>
       <c r="H32" s="24">
         <f t="shared" si="14"/>
-        <v>0.5</v>
+        <v>-21338.7</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="15"/>
-        <v>0.5</v>
+        <v>21338.7</v>
       </c>
       <c r="K32" s="7"/>
       <c r="L32" s="24">
@@ -6715,27 +6307,23 @@
       <c r="A33" s="5">
         <v>21540.1</v>
       </c>
-      <c r="C33" s="20">
-        <v>21540.799999999999</v>
-      </c>
+      <c r="C33" s="20"/>
       <c r="D33" s="24">
         <f t="shared" si="12"/>
-        <v>0.7000000000007276</v>
+        <v>-21540.1</v>
       </c>
       <c r="E33" s="9">
         <f t="shared" si="13"/>
-        <v>0.7000000000007276</v>
-      </c>
-      <c r="G33" s="54">
-        <v>21541.3</v>
-      </c>
+        <v>21540.1</v>
+      </c>
+      <c r="G33" s="44"/>
       <c r="H33" s="24">
         <f t="shared" si="14"/>
-        <v>1.2000000000007276</v>
+        <v>-21540.1</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="15"/>
-        <v>1.2000000000007276</v>
+        <v>21540.1</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="24">
@@ -6751,27 +6339,23 @@
       <c r="A34" s="5">
         <v>22083.200000000001</v>
       </c>
-      <c r="C34" s="20">
-        <v>22083.8</v>
-      </c>
+      <c r="C34" s="20"/>
       <c r="D34" s="24">
         <f t="shared" si="12"/>
-        <v>0.59999999999854481</v>
+        <v>-22083.200000000001</v>
       </c>
       <c r="E34" s="9">
         <f t="shared" si="13"/>
-        <v>0.59999999999854481</v>
-      </c>
-      <c r="G34" s="54">
-        <v>22084.1</v>
-      </c>
+        <v>22083.200000000001</v>
+      </c>
+      <c r="G34" s="44"/>
       <c r="H34" s="24">
         <f t="shared" si="14"/>
-        <v>0.89999999999781721</v>
+        <v>-22083.200000000001</v>
       </c>
       <c r="I34" s="9">
         <f t="shared" si="15"/>
-        <v>0.89999999999781721</v>
+        <v>22083.200000000001</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="24">
@@ -6787,27 +6371,23 @@
       <c r="A35" s="5">
         <v>23139.5</v>
       </c>
-      <c r="C35" s="20">
-        <v>23140.1</v>
-      </c>
+      <c r="C35" s="20"/>
       <c r="D35" s="24">
         <f t="shared" si="12"/>
-        <v>0.59999999999854481</v>
+        <v>-23139.5</v>
       </c>
       <c r="E35" s="9">
         <f t="shared" si="13"/>
-        <v>0.59999999999854481</v>
-      </c>
-      <c r="G35" s="54">
-        <v>23139.9</v>
-      </c>
+        <v>23139.5</v>
+      </c>
+      <c r="G35" s="44"/>
       <c r="H35" s="24">
         <f t="shared" si="14"/>
-        <v>0.40000000000145519</v>
+        <v>-23139.5</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" si="15"/>
-        <v>0.40000000000145519</v>
+        <v>23139.5</v>
       </c>
       <c r="K35" s="7"/>
       <c r="L35" s="24">
@@ -6823,27 +6403,23 @@
       <c r="A36" s="5">
         <v>23851.5</v>
       </c>
-      <c r="C36" s="20">
-        <v>23847.9</v>
-      </c>
+      <c r="C36" s="20"/>
       <c r="D36" s="24">
         <f t="shared" si="12"/>
-        <v>-3.5999999999985448</v>
+        <v>-23851.5</v>
       </c>
       <c r="E36" s="9">
         <f t="shared" si="13"/>
-        <v>3.5999999999985448</v>
-      </c>
-      <c r="G36" s="54">
-        <v>23853.599999999999</v>
-      </c>
+        <v>23851.5</v>
+      </c>
+      <c r="G36" s="44"/>
       <c r="H36" s="24">
         <f t="shared" si="14"/>
-        <v>2.0999999999985448</v>
+        <v>-23851.5</v>
       </c>
       <c r="I36" s="9">
         <f t="shared" si="15"/>
-        <v>2.0999999999985448</v>
+        <v>23851.5</v>
       </c>
       <c r="K36" s="7"/>
       <c r="L36" s="24">
@@ -6859,27 +6435,23 @@
       <c r="A37" s="5">
         <v>23973.1</v>
       </c>
-      <c r="C37" s="20">
-        <v>23972.7</v>
-      </c>
+      <c r="C37" s="20"/>
       <c r="D37" s="24">
         <f t="shared" si="12"/>
-        <v>-0.39999999999781721</v>
+        <v>-23973.1</v>
       </c>
       <c r="E37" s="9">
         <f t="shared" si="13"/>
-        <v>0.39999999999781721</v>
-      </c>
-      <c r="G37" s="54">
-        <v>23972.9</v>
-      </c>
+        <v>23973.1</v>
+      </c>
+      <c r="G37" s="44"/>
       <c r="H37" s="24">
         <f t="shared" si="14"/>
-        <v>-0.19999999999708962</v>
+        <v>-23973.1</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="15"/>
-        <v>0.19999999999708962</v>
+        <v>23973.1</v>
       </c>
       <c r="K37" s="7"/>
       <c r="L37" s="24">
@@ -6919,11 +6491,11 @@
       </c>
       <c r="D40" s="24">
         <f>AVERAGE(D14:D37)</f>
-        <v>-0.6043478260867825</v>
+        <v>-18583.304347826084</v>
       </c>
       <c r="E40" s="10">
         <f>AVERAGE(E14:E37)</f>
-        <v>1.0391304347821184</v>
+        <v>18583.304347826084</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="24" t="s">
@@ -6931,11 +6503,11 @@
       </c>
       <c r="H40" s="24">
         <f>AVERAGE(H14:H37)</f>
-        <v>-0.13913043478232398</v>
+        <v>-18583.304347826084</v>
       </c>
       <c r="I40" s="10">
         <f>AVERAGE(I14:I37)</f>
-        <v>0.8173913043481108</v>
+        <v>18583.304347826084</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>67</v>
@@ -6955,11 +6527,11 @@
       </c>
       <c r="D41" s="24">
         <f>STDEV(D14:D37)</f>
-        <v>1.2426065935136972</v>
+        <v>3374.4307066631636</v>
       </c>
       <c r="E41" s="10">
         <f>STDEV(E14:E37)</f>
-        <v>0.89276848797548336</v>
+        <v>3374.4307066631636</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="24" t="s">
@@ -6967,11 +6539,11 @@
       </c>
       <c r="H41" s="24">
         <f>STDEV(H14:H37)</f>
-        <v>1.0798733639707812</v>
+        <v>3374.4307066631636</v>
       </c>
       <c r="I41" s="10">
         <f>STDEV(I14:I37)</f>
-        <v>0.69847377377234743</v>
+        <v>3374.4307066631636</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>68</v>

</xml_diff>